<commit_message>
Added AD-64 Log Handling, incomplete
</commit_message>
<xml_diff>
--- a/Projects/Sung/Mapping Data/RTI Diagnostics Feed Info - Sung.xlsx
+++ b/Projects/Sung/Mapping Data/RTI Diagnostics Feed Info - Sung.xlsx
@@ -8,9 +8,8 @@
     <sheet state="visible" name="Source List" sheetId="3" r:id="rId6"/>
     <sheet state="visible" name="Audio Zones" sheetId="4" r:id="rId7"/>
     <sheet state="visible" name="Video Zones" sheetId="5" r:id="rId8"/>
-    <sheet state="visible" name="RCM12 List" sheetId="6" r:id="rId9"/>
-    <sheet state="visible" name="Ports List" sheetId="7" r:id="rId10"/>
-    <sheet state="visible" name="Lighting Loads" sheetId="8" r:id="rId11"/>
+    <sheet state="visible" name="Ports List" sheetId="6" r:id="rId9"/>
+    <sheet state="visible" name="Lighting Loads" sheetId="7" r:id="rId10"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -18,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="761" uniqueCount="423">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="746" uniqueCount="420">
   <si>
     <t>Room Index</t>
   </si>
@@ -176,9 +175,6 @@
     <t>Apple TV 1 - House (Global &gt; Apple TV #1 (Gen 4))</t>
   </si>
   <si>
-    <t>Apple TV 2 - Room (Global &gt; Apple TV #2 Gen 4))</t>
-  </si>
-  <si>
     <t>Apple TV 2 - Room (Global &gt; Apple TV #2 (Gen 4))</t>
   </si>
   <si>
@@ -881,10 +877,154 @@
     <t>Sonos Port 2</t>
   </si>
   <si>
-    <t>Relay Index</t>
-  </si>
-  <si>
-    <t>Relay Name</t>
+    <t>Module Name</t>
+  </si>
+  <si>
+    <t>Module Type</t>
+  </si>
+  <si>
+    <t>Port Index</t>
+  </si>
+  <si>
+    <t>Port Name</t>
+  </si>
+  <si>
+    <t>XP-8v</t>
+  </si>
+  <si>
+    <t>Internal MPIO</t>
+  </si>
+  <si>
+    <t>MPIO 1</t>
+  </si>
+  <si>
+    <t>MPIO 2</t>
+  </si>
+  <si>
+    <t>MPIO 3</t>
+  </si>
+  <si>
+    <t>MPIO 4</t>
+  </si>
+  <si>
+    <t>MPIO 5</t>
+  </si>
+  <si>
+    <t>MPIO 6</t>
+  </si>
+  <si>
+    <t>MPIO 7</t>
+  </si>
+  <si>
+    <t>MPIO 8</t>
+  </si>
+  <si>
+    <t>Internal Relay</t>
+  </si>
+  <si>
+    <t>Relay 1</t>
+  </si>
+  <si>
+    <t>Relay 2</t>
+  </si>
+  <si>
+    <t>Relay 3</t>
+  </si>
+  <si>
+    <t>Relay 4</t>
+  </si>
+  <si>
+    <t>Relay 5</t>
+  </si>
+  <si>
+    <t>Relay 6</t>
+  </si>
+  <si>
+    <t>Relay 7</t>
+  </si>
+  <si>
+    <t>Relay 8</t>
+  </si>
+  <si>
+    <t>XP8v</t>
+  </si>
+  <si>
+    <t>Internal Sense</t>
+  </si>
+  <si>
+    <t>Sense 1</t>
+  </si>
+  <si>
+    <t>Sense 2</t>
+  </si>
+  <si>
+    <t>Sense 3</t>
+  </si>
+  <si>
+    <t>Sense 4</t>
+  </si>
+  <si>
+    <t>Sense 5</t>
+  </si>
+  <si>
+    <t>Sense 6</t>
+  </si>
+  <si>
+    <t>Sense 7</t>
+  </si>
+  <si>
+    <t>Sense 8</t>
+  </si>
+  <si>
+    <t>Internal RS232</t>
+  </si>
+  <si>
+    <t>RS232 1</t>
+  </si>
+  <si>
+    <t>RS232 2</t>
+  </si>
+  <si>
+    <t>RS232 3</t>
+  </si>
+  <si>
+    <t>RS232 4</t>
+  </si>
+  <si>
+    <t>RS232 5</t>
+  </si>
+  <si>
+    <t>RS232 6</t>
+  </si>
+  <si>
+    <t>RS232 7</t>
+  </si>
+  <si>
+    <t>RS232 8</t>
+  </si>
+  <si>
+    <t>XP-6</t>
+  </si>
+  <si>
+    <t>Internal Trigger</t>
+  </si>
+  <si>
+    <t>Trigger 1</t>
+  </si>
+  <si>
+    <t>Trigger 2</t>
+  </si>
+  <si>
+    <t>Trigger 3</t>
+  </si>
+  <si>
+    <t>ESC-2</t>
+  </si>
+  <si>
+    <t>RCM-4</t>
+  </si>
+  <si>
+    <t>RCM-12</t>
   </si>
   <si>
     <t>HRV Main Fan</t>
@@ -918,156 +1058,6 @@
   </si>
   <si>
     <t>Spare</t>
-  </si>
-  <si>
-    <t>Module Name</t>
-  </si>
-  <si>
-    <t>Module Type</t>
-  </si>
-  <si>
-    <t>Port Index</t>
-  </si>
-  <si>
-    <t>Port Name</t>
-  </si>
-  <si>
-    <t>XP-8v</t>
-  </si>
-  <si>
-    <t>Internal MPIO</t>
-  </si>
-  <si>
-    <t>MPIO 1</t>
-  </si>
-  <si>
-    <t>MPIO 2</t>
-  </si>
-  <si>
-    <t>MPIO 3</t>
-  </si>
-  <si>
-    <t>MPIO 4</t>
-  </si>
-  <si>
-    <t>MPIO 5</t>
-  </si>
-  <si>
-    <t>MPIO 6</t>
-  </si>
-  <si>
-    <t>MPIO 7</t>
-  </si>
-  <si>
-    <t>MPIO 8</t>
-  </si>
-  <si>
-    <t>Internal Relay</t>
-  </si>
-  <si>
-    <t>Relay 1</t>
-  </si>
-  <si>
-    <t>Relay 2</t>
-  </si>
-  <si>
-    <t>Relay 3</t>
-  </si>
-  <si>
-    <t>Relay 4</t>
-  </si>
-  <si>
-    <t>Relay 5</t>
-  </si>
-  <si>
-    <t>Relay 6</t>
-  </si>
-  <si>
-    <t>Relay 7</t>
-  </si>
-  <si>
-    <t>Relay 8</t>
-  </si>
-  <si>
-    <t>XP8v</t>
-  </si>
-  <si>
-    <t>Internal Sense</t>
-  </si>
-  <si>
-    <t>Sense 1</t>
-  </si>
-  <si>
-    <t>Sense 2</t>
-  </si>
-  <si>
-    <t>Sense 3</t>
-  </si>
-  <si>
-    <t>Sense 4</t>
-  </si>
-  <si>
-    <t>Sense 5</t>
-  </si>
-  <si>
-    <t>Sense 6</t>
-  </si>
-  <si>
-    <t>Sense 7</t>
-  </si>
-  <si>
-    <t>Sense 8</t>
-  </si>
-  <si>
-    <t>Internal RS232</t>
-  </si>
-  <si>
-    <t>RS232 1</t>
-  </si>
-  <si>
-    <t>RS232 2</t>
-  </si>
-  <si>
-    <t>RS232 3</t>
-  </si>
-  <si>
-    <t>RS232 4</t>
-  </si>
-  <si>
-    <t>RS232 5</t>
-  </si>
-  <si>
-    <t>RS232 6</t>
-  </si>
-  <si>
-    <t>RS232 7</t>
-  </si>
-  <si>
-    <t>RS232 8</t>
-  </si>
-  <si>
-    <t>XP-6</t>
-  </si>
-  <si>
-    <t>Internal Trigger</t>
-  </si>
-  <si>
-    <t>Trigger 1</t>
-  </si>
-  <si>
-    <t>Trigger 2</t>
-  </si>
-  <si>
-    <t>Trigger 3</t>
-  </si>
-  <si>
-    <t>ESC-2</t>
-  </si>
-  <si>
-    <t>RCM-4</t>
-  </si>
-  <si>
-    <t>RCM-12</t>
   </si>
   <si>
     <t>Load Index</t>
@@ -1349,14 +1339,14 @@
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" vertical="bottom"/>
-    </xf>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" vertical="bottom"/>
     </xf>
     <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0"/>
@@ -1395,10 +1385,6 @@
 </file>
 
 <file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing8.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
@@ -2940,14 +2926,6 @@
         <v>165</v>
       </c>
     </row>
-    <row r="139">
-      <c r="A139" s="3">
-        <v>138.0</v>
-      </c>
-      <c r="B139" s="1" t="s">
-        <v>166</v>
-      </c>
-    </row>
   </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>
@@ -2969,10 +2947,10 @@
     <row r="1">
       <c r="A1" s="4"/>
       <c r="B1" s="4" t="s">
+        <v>166</v>
+      </c>
+      <c r="C1" s="4" t="s">
         <v>167</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>168</v>
       </c>
     </row>
     <row r="2">
@@ -2983,7 +2961,7 @@
         <v>0.0</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="3">
@@ -2994,7 +2972,7 @@
         <v>1.0</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="4">
@@ -3005,7 +2983,7 @@
         <v>2.0</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="5">
@@ -3016,7 +2994,7 @@
         <v>3.0</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="6">
@@ -3027,7 +3005,7 @@
         <v>4.0</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="7">
@@ -3038,7 +3016,7 @@
         <v>5.0</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="8">
@@ -3049,7 +3027,7 @@
         <v>6.0</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="9">
@@ -3060,7 +3038,7 @@
         <v>7.0</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="10">
@@ -3071,7 +3049,7 @@
         <v>8.0</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="11">
@@ -3082,7 +3060,7 @@
         <v>9.0</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="12">
@@ -3093,7 +3071,7 @@
         <v>10.0</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="13">
@@ -3104,7 +3082,7 @@
         <v>11.0</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="14">
@@ -3115,7 +3093,7 @@
         <v>12.0</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="15">
@@ -3126,7 +3104,7 @@
         <v>13.0</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="16">
@@ -3137,7 +3115,7 @@
         <v>14.0</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="17">
@@ -3148,7 +3126,7 @@
         <v>15.0</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="18">
@@ -3159,7 +3137,7 @@
         <v>16.0</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="19">
@@ -3170,7 +3148,7 @@
         <v>17.0</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="20">
@@ -3181,7 +3159,7 @@
         <v>18.0</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="21">
@@ -3192,7 +3170,7 @@
         <v>19.0</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="22">
@@ -3203,7 +3181,7 @@
         <v>20.0</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="23">
@@ -3214,7 +3192,7 @@
         <v>21.0</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="24">
@@ -3225,7 +3203,7 @@
         <v>22.0</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="25">
@@ -3236,7 +3214,7 @@
         <v>23.0</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="26">
@@ -3247,7 +3225,7 @@
         <v>24.0</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="27">
@@ -3258,7 +3236,7 @@
         <v>25.0</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="28">
@@ -3269,7 +3247,7 @@
         <v>26.0</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="29">
@@ -3280,7 +3258,7 @@
         <v>27.0</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="30">
@@ -3291,7 +3269,7 @@
         <v>28.0</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="31">
@@ -3302,7 +3280,7 @@
         <v>29.0</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="32">
@@ -3313,7 +3291,7 @@
         <v>30.0</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="33">
@@ -3324,7 +3302,7 @@
         <v>31.0</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="34">
@@ -3335,7 +3313,7 @@
         <v>32.0</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="35">
@@ -3346,7 +3324,7 @@
         <v>33.0</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="36">
@@ -3357,7 +3335,7 @@
         <v>34.0</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="37">
@@ -3368,7 +3346,7 @@
         <v>35.0</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="38">
@@ -3379,7 +3357,7 @@
         <v>36.0</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="39">
@@ -3390,7 +3368,7 @@
         <v>37.0</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="40">
@@ -3401,7 +3379,7 @@
         <v>38.0</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="41">
@@ -3412,7 +3390,7 @@
         <v>39.0</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="42">
@@ -3423,7 +3401,7 @@
         <v>40.0</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="43">
@@ -3434,7 +3412,7 @@
         <v>41.0</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="44">
@@ -3445,7 +3423,7 @@
         <v>42.0</v>
       </c>
       <c r="C44" s="4" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="45">
@@ -3456,7 +3434,7 @@
         <v>43.0</v>
       </c>
       <c r="C45" s="4" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="46">
@@ -3467,7 +3445,7 @@
         <v>44.0</v>
       </c>
       <c r="C46" s="4" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="47">
@@ -3478,7 +3456,7 @@
         <v>45.0</v>
       </c>
       <c r="C47" s="4" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="48">
@@ -3489,7 +3467,7 @@
         <v>46.0</v>
       </c>
       <c r="C48" s="4" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="49">
@@ -3500,7 +3478,7 @@
         <v>47.0</v>
       </c>
       <c r="C49" s="4" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="50">
@@ -3511,7 +3489,7 @@
         <v>48.0</v>
       </c>
       <c r="C50" s="4" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="51">
@@ -3522,7 +3500,7 @@
         <v>49.0</v>
       </c>
       <c r="C51" s="4" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="52">
@@ -3533,7 +3511,7 @@
         <v>50.0</v>
       </c>
       <c r="C52" s="4" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="53">
@@ -3544,7 +3522,7 @@
         <v>51.0</v>
       </c>
       <c r="C53" s="4" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="54">
@@ -3555,7 +3533,7 @@
         <v>52.0</v>
       </c>
       <c r="C54" s="4" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="55">
@@ -3566,7 +3544,7 @@
         <v>53.0</v>
       </c>
       <c r="C55" s="4" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="56">
@@ -3577,7 +3555,7 @@
         <v>54.0</v>
       </c>
       <c r="C56" s="4" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="57">
@@ -3588,7 +3566,7 @@
         <v>55.0</v>
       </c>
       <c r="C57" s="4" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="58">
@@ -3599,7 +3577,7 @@
         <v>56.0</v>
       </c>
       <c r="C58" s="4" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="59">
@@ -3610,7 +3588,7 @@
         <v>57.0</v>
       </c>
       <c r="C59" s="4" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="60">
@@ -3621,7 +3599,7 @@
         <v>58.0</v>
       </c>
       <c r="C60" s="4" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="61">
@@ -3632,7 +3610,7 @@
         <v>59.0</v>
       </c>
       <c r="C61" s="4" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="62">
@@ -3643,7 +3621,7 @@
         <v>60.0</v>
       </c>
       <c r="C62" s="4" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="63">
@@ -3654,7 +3632,7 @@
         <v>61.0</v>
       </c>
       <c r="C63" s="4" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="64">
@@ -3665,7 +3643,7 @@
         <v>62.0</v>
       </c>
       <c r="C64" s="4" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="65">
@@ -3676,7 +3654,7 @@
         <v>63.0</v>
       </c>
       <c r="C65" s="4" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="66">
@@ -3687,7 +3665,7 @@
         <v>64.0</v>
       </c>
       <c r="C66" s="4" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="67">
@@ -3698,7 +3676,7 @@
         <v>65.0</v>
       </c>
       <c r="C67" s="4" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="68">
@@ -3709,7 +3687,7 @@
         <v>66.0</v>
       </c>
       <c r="C68" s="4" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="69">
@@ -3720,7 +3698,7 @@
         <v>67.0</v>
       </c>
       <c r="C69" s="4" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="70">
@@ -3731,7 +3709,7 @@
         <v>68.0</v>
       </c>
       <c r="C70" s="4" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="71">
@@ -3742,7 +3720,7 @@
         <v>69.0</v>
       </c>
       <c r="C71" s="4" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="72">
@@ -3753,7 +3731,7 @@
         <v>70.0</v>
       </c>
       <c r="C72" s="4" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="73">
@@ -3764,7 +3742,7 @@
         <v>71.0</v>
       </c>
       <c r="C73" s="4" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="74">
@@ -3775,7 +3753,7 @@
         <v>72.0</v>
       </c>
       <c r="C74" s="4" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="75">
@@ -3786,7 +3764,7 @@
         <v>73.0</v>
       </c>
       <c r="C75" s="4" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="76">
@@ -3797,7 +3775,7 @@
         <v>74.0</v>
       </c>
       <c r="C76" s="4" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="77">
@@ -3808,7 +3786,7 @@
         <v>75.0</v>
       </c>
       <c r="C77" s="4" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="78">
@@ -3819,7 +3797,7 @@
         <v>76.0</v>
       </c>
       <c r="C78" s="4" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="79">
@@ -3830,7 +3808,7 @@
         <v>77.0</v>
       </c>
       <c r="C79" s="4" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="80">
@@ -3841,7 +3819,7 @@
         <v>78.0</v>
       </c>
       <c r="C80" s="4" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="81">
@@ -3852,7 +3830,7 @@
         <v>79.0</v>
       </c>
       <c r="C81" s="4" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="82">
@@ -3863,7 +3841,7 @@
         <v>80.0</v>
       </c>
       <c r="C82" s="4" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="83">
@@ -3874,7 +3852,7 @@
         <v>81.0</v>
       </c>
       <c r="C83" s="4" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="84">
@@ -3885,7 +3863,7 @@
         <v>82.0</v>
       </c>
       <c r="C84" s="4" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="85">
@@ -3896,7 +3874,7 @@
         <v>83.0</v>
       </c>
       <c r="C85" s="4" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="86">
@@ -3907,7 +3885,7 @@
         <v>84.0</v>
       </c>
       <c r="C86" s="4" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="87">
@@ -3918,7 +3896,7 @@
         <v>85.0</v>
       </c>
       <c r="C87" s="4" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="88">
@@ -3929,7 +3907,7 @@
         <v>86.0</v>
       </c>
       <c r="C88" s="4" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="89">
@@ -3940,7 +3918,7 @@
         <v>87.0</v>
       </c>
       <c r="C89" s="4" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="90">
@@ -3951,7 +3929,7 @@
         <v>88.0</v>
       </c>
       <c r="C90" s="4" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="91">
@@ -3962,7 +3940,7 @@
         <v>89.0</v>
       </c>
       <c r="C91" s="4" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="92">
@@ -3973,7 +3951,7 @@
         <v>90.0</v>
       </c>
       <c r="C92" s="4" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="93">
@@ -3984,7 +3962,7 @@
         <v>91.0</v>
       </c>
       <c r="C93" s="4" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="94">
@@ -3995,7 +3973,7 @@
         <v>92.0</v>
       </c>
       <c r="C94" s="4" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="95">
@@ -4006,7 +3984,7 @@
         <v>93.0</v>
       </c>
       <c r="C95" s="4" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="96">
@@ -4017,7 +3995,7 @@
         <v>94.0</v>
       </c>
       <c r="C96" s="4" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="97">
@@ -4028,7 +4006,7 @@
         <v>95.0</v>
       </c>
       <c r="C97" s="4" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="98">
@@ -4039,7 +4017,7 @@
         <v>96.0</v>
       </c>
       <c r="C98" s="4" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="99">
@@ -4050,7 +4028,7 @@
         <v>97.0</v>
       </c>
       <c r="C99" s="4" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="100">
@@ -4061,7 +4039,7 @@
         <v>98.0</v>
       </c>
       <c r="C100" s="4" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="101">
@@ -4072,7 +4050,7 @@
         <v>99.0</v>
       </c>
       <c r="C101" s="4" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="102">
@@ -4083,7 +4061,7 @@
         <v>100.0</v>
       </c>
       <c r="C102" s="4" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="103">
@@ -4094,7 +4072,7 @@
         <v>101.0</v>
       </c>
       <c r="C103" s="4" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="104">
@@ -4105,7 +4083,7 @@
         <v>102.0</v>
       </c>
       <c r="C104" s="4" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="105">
@@ -4116,7 +4094,7 @@
         <v>103.0</v>
       </c>
       <c r="C105" s="4" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="106">
@@ -4127,7 +4105,7 @@
         <v>104.0</v>
       </c>
       <c r="C106" s="4" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="107">
@@ -4138,7 +4116,7 @@
         <v>105.0</v>
       </c>
       <c r="C107" s="4" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="108">
@@ -4149,7 +4127,7 @@
         <v>106.0</v>
       </c>
       <c r="C108" s="4" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="109">
@@ -4160,7 +4138,7 @@
         <v>107.0</v>
       </c>
       <c r="C109" s="4" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="110">
@@ -4171,7 +4149,7 @@
         <v>108.0</v>
       </c>
       <c r="C110" s="4" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="111">
@@ -4182,7 +4160,7 @@
         <v>109.0</v>
       </c>
       <c r="C111" s="4" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="112">
@@ -4193,7 +4171,7 @@
         <v>110.0</v>
       </c>
       <c r="C112" s="4" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="113">
@@ -4204,7 +4182,7 @@
         <v>111.0</v>
       </c>
       <c r="C113" s="4" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="114">
@@ -4215,7 +4193,7 @@
         <v>112.0</v>
       </c>
       <c r="C114" s="4" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="115">
@@ -4226,7 +4204,7 @@
         <v>113.0</v>
       </c>
       <c r="C115" s="4" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="116">
@@ -4237,7 +4215,7 @@
         <v>114.0</v>
       </c>
       <c r="C116" s="4" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="117">
@@ -4248,7 +4226,7 @@
         <v>115.0</v>
       </c>
       <c r="C117" s="4" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="118">
@@ -4259,7 +4237,7 @@
         <v>116.0</v>
       </c>
       <c r="C118" s="4" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="119">
@@ -4270,7 +4248,7 @@
         <v>117.0</v>
       </c>
       <c r="C119" s="4" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="120">
@@ -4281,7 +4259,7 @@
         <v>118.0</v>
       </c>
       <c r="C120" s="4" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="121">
@@ -4292,7 +4270,7 @@
         <v>119.0</v>
       </c>
       <c r="C121" s="4" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="122">
@@ -4303,7 +4281,7 @@
         <v>120.0</v>
       </c>
       <c r="C122" s="4" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="123">
@@ -4314,7 +4292,7 @@
         <v>121.0</v>
       </c>
       <c r="C123" s="4" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="124">
@@ -4325,7 +4303,7 @@
         <v>122.0</v>
       </c>
       <c r="C124" s="4" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="125">
@@ -4336,7 +4314,7 @@
         <v>123.0</v>
       </c>
       <c r="C125" s="4" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="126">
@@ -4347,7 +4325,7 @@
         <v>124.0</v>
       </c>
       <c r="C126" s="4" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="127">
@@ -4358,7 +4336,7 @@
         <v>125.0</v>
       </c>
       <c r="C127" s="4" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="128">
@@ -4369,7 +4347,7 @@
         <v>126.0</v>
       </c>
       <c r="C128" s="4" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="129">
@@ -4380,7 +4358,7 @@
         <v>127.0</v>
       </c>
       <c r="C129" s="4" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="130">
@@ -4391,7 +4369,7 @@
         <v>128.0</v>
       </c>
       <c r="C130" s="4" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="131">
@@ -4402,7 +4380,7 @@
         <v>129.0</v>
       </c>
       <c r="C131" s="4" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
   </sheetData>
@@ -4428,16 +4406,16 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="4" t="s">
+        <v>271</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>272</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="C1" s="4" t="s">
         <v>273</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="D1" s="4" t="s">
         <v>274</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>275</v>
       </c>
     </row>
     <row r="2">
@@ -4445,13 +4423,13 @@
         <v>1.0</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="C2" s="4">
         <v>1.0</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="3">
@@ -4459,13 +4437,13 @@
         <v>2.0</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C3" s="4">
         <v>2.0</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="4">
@@ -4473,7 +4451,7 @@
         <v>3.0</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="C4" s="4">
         <v>3.0</v>
@@ -4495,7 +4473,7 @@
         <v>5.0</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="C6" s="4">
         <v>5.0</v>
@@ -4509,7 +4487,7 @@
         <v>6.0</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="C7" s="4">
         <v>6.0</v>
@@ -4523,7 +4501,7 @@
         <v>7.0</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="C8" s="4">
         <v>7.0</v>
@@ -4537,7 +4515,7 @@
         <v>8.0</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C9" s="4">
         <v>8.0</v>
@@ -4551,7 +4529,7 @@
         <v>9.0</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="C10" s="4">
         <v>9.0</v>
@@ -4565,7 +4543,7 @@
         <v>10.0</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C11" s="4">
         <v>10.0</v>
@@ -4659,128 +4637,6 @@
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
-  <cols>
-    <col customWidth="1" min="2" max="2" width="15.63"/>
-  </cols>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="2" t="s">
-        <v>287</v>
-      </c>
-      <c r="B1" s="5" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="3">
-        <v>1.0</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="3">
-        <v>2.0</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="3">
-        <v>3.0</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="3">
-        <v>4.0</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="3">
-        <v>5.0</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="3">
-        <v>6.0</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="3">
-        <v>7.0</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="3">
-        <v>8.0</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="3">
-        <v>9.0</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" s="3">
-        <v>10.0</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" s="3">
-        <v>11.0</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" s="3">
-        <v>12.0</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>299</v>
-      </c>
-    </row>
-  </sheetData>
-  <drawing r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="0" summaryRight="0"/>
-  </sheetPr>
-  <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1.0" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B3" sqref="B3" pane="bottomLeft"/>
@@ -4793,128 +4649,128 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>300</v>
+        <v>286</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>301</v>
+        <v>287</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>302</v>
+        <v>288</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>303</v>
+        <v>289</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="6" t="s">
-        <v>304</v>
+      <c r="A2" s="5" t="s">
+        <v>290</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>305</v>
+        <v>291</v>
       </c>
       <c r="C2" s="3">
         <v>1.0</v>
       </c>
-      <c r="D2" s="7" t="s">
-        <v>306</v>
+      <c r="D2" s="6" t="s">
+        <v>292</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="6" t="s">
-        <v>304</v>
+      <c r="A3" s="5" t="s">
+        <v>290</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>305</v>
+        <v>291</v>
       </c>
       <c r="C3" s="3">
         <v>2.0</v>
       </c>
-      <c r="D3" s="7" t="s">
-        <v>307</v>
+      <c r="D3" s="6" t="s">
+        <v>293</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="6" t="s">
-        <v>304</v>
+      <c r="A4" s="5" t="s">
+        <v>290</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>305</v>
+        <v>291</v>
       </c>
       <c r="C4" s="3">
         <v>3.0</v>
       </c>
-      <c r="D4" s="7" t="s">
-        <v>308</v>
+      <c r="D4" s="6" t="s">
+        <v>294</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="6" t="s">
-        <v>304</v>
+      <c r="A5" s="5" t="s">
+        <v>290</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>305</v>
+        <v>291</v>
       </c>
       <c r="C5" s="3">
         <v>4.0</v>
       </c>
-      <c r="D5" s="7" t="s">
-        <v>309</v>
+      <c r="D5" s="6" t="s">
+        <v>295</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="6" t="s">
-        <v>304</v>
+      <c r="A6" s="5" t="s">
+        <v>290</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>305</v>
+        <v>291</v>
       </c>
       <c r="C6" s="3">
         <v>5.0</v>
       </c>
-      <c r="D6" s="7" t="s">
-        <v>310</v>
+      <c r="D6" s="6" t="s">
+        <v>296</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="6" t="s">
-        <v>304</v>
+      <c r="A7" s="5" t="s">
+        <v>290</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>305</v>
+        <v>291</v>
       </c>
       <c r="C7" s="3">
         <v>6.0</v>
       </c>
-      <c r="D7" s="7" t="s">
-        <v>311</v>
+      <c r="D7" s="6" t="s">
+        <v>297</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="6" t="s">
-        <v>304</v>
+      <c r="A8" s="5" t="s">
+        <v>290</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>305</v>
+        <v>291</v>
       </c>
       <c r="C8" s="3">
         <v>7.0</v>
       </c>
-      <c r="D8" s="7" t="s">
-        <v>312</v>
+      <c r="D8" s="6" t="s">
+        <v>298</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="6" t="s">
-        <v>304</v>
+      <c r="A9" s="5" t="s">
+        <v>290</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>305</v>
+        <v>291</v>
       </c>
       <c r="C9" s="3">
         <v>8.0</v>
       </c>
-      <c r="D9" s="7" t="s">
-        <v>313</v>
+      <c r="D9" s="6" t="s">
+        <v>299</v>
       </c>
     </row>
     <row r="10">
@@ -4924,115 +4780,115 @@
       <c r="D10" s="1"/>
     </row>
     <row r="11">
-      <c r="A11" s="6" t="s">
-        <v>304</v>
+      <c r="A11" s="5" t="s">
+        <v>290</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>314</v>
+        <v>300</v>
       </c>
       <c r="C11" s="3">
         <v>1.0</v>
       </c>
-      <c r="D11" s="7" t="s">
-        <v>315</v>
+      <c r="D11" s="6" t="s">
+        <v>301</v>
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="6" t="s">
-        <v>304</v>
+      <c r="A12" s="5" t="s">
+        <v>290</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>314</v>
+        <v>300</v>
       </c>
       <c r="C12" s="3">
         <v>2.0</v>
       </c>
-      <c r="D12" s="7" t="s">
-        <v>316</v>
+      <c r="D12" s="6" t="s">
+        <v>302</v>
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="6" t="s">
-        <v>304</v>
+      <c r="A13" s="5" t="s">
+        <v>290</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>314</v>
+        <v>300</v>
       </c>
       <c r="C13" s="3">
         <v>3.0</v>
       </c>
-      <c r="D13" s="7" t="s">
-        <v>317</v>
+      <c r="D13" s="6" t="s">
+        <v>303</v>
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="6" t="s">
-        <v>304</v>
+      <c r="A14" s="5" t="s">
+        <v>290</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>314</v>
+        <v>300</v>
       </c>
       <c r="C14" s="3">
         <v>4.0</v>
       </c>
-      <c r="D14" s="7" t="s">
-        <v>318</v>
+      <c r="D14" s="6" t="s">
+        <v>304</v>
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="6" t="s">
-        <v>304</v>
+      <c r="A15" s="5" t="s">
+        <v>290</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>314</v>
+        <v>300</v>
       </c>
       <c r="C15" s="3">
         <v>5.0</v>
       </c>
-      <c r="D15" s="7" t="s">
-        <v>319</v>
+      <c r="D15" s="6" t="s">
+        <v>305</v>
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="6" t="s">
-        <v>304</v>
+      <c r="A16" s="5" t="s">
+        <v>290</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>314</v>
+        <v>300</v>
       </c>
       <c r="C16" s="3">
         <v>6.0</v>
       </c>
-      <c r="D16" s="7" t="s">
-        <v>320</v>
+      <c r="D16" s="6" t="s">
+        <v>306</v>
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="6" t="s">
-        <v>304</v>
+      <c r="A17" s="5" t="s">
+        <v>290</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>314</v>
+        <v>300</v>
       </c>
       <c r="C17" s="3">
         <v>7.0</v>
       </c>
-      <c r="D17" s="7" t="s">
-        <v>321</v>
+      <c r="D17" s="6" t="s">
+        <v>307</v>
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="6" t="s">
-        <v>304</v>
+      <c r="A18" s="5" t="s">
+        <v>290</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>314</v>
+        <v>300</v>
       </c>
       <c r="C18" s="3">
         <v>8.0</v>
       </c>
-      <c r="D18" s="7" t="s">
-        <v>322</v>
+      <c r="D18" s="6" t="s">
+        <v>308</v>
       </c>
     </row>
     <row r="19">
@@ -5042,115 +4898,115 @@
       <c r="D19" s="1"/>
     </row>
     <row r="20">
-      <c r="A20" s="6" t="s">
-        <v>323</v>
+      <c r="A20" s="5" t="s">
+        <v>309</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>324</v>
+        <v>310</v>
       </c>
       <c r="C20" s="3">
         <v>1.0</v>
       </c>
-      <c r="D20" s="7" t="s">
-        <v>325</v>
+      <c r="D20" s="6" t="s">
+        <v>311</v>
       </c>
     </row>
     <row r="21">
-      <c r="A21" s="6" t="s">
-        <v>323</v>
+      <c r="A21" s="5" t="s">
+        <v>309</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>324</v>
+        <v>310</v>
       </c>
       <c r="C21" s="3">
         <v>2.0</v>
       </c>
-      <c r="D21" s="7" t="s">
-        <v>326</v>
+      <c r="D21" s="6" t="s">
+        <v>312</v>
       </c>
     </row>
     <row r="22">
-      <c r="A22" s="6" t="s">
-        <v>323</v>
+      <c r="A22" s="5" t="s">
+        <v>309</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>324</v>
+        <v>310</v>
       </c>
       <c r="C22" s="3">
         <v>3.0</v>
       </c>
-      <c r="D22" s="7" t="s">
-        <v>327</v>
+      <c r="D22" s="6" t="s">
+        <v>313</v>
       </c>
     </row>
     <row r="23">
-      <c r="A23" s="6" t="s">
-        <v>323</v>
+      <c r="A23" s="5" t="s">
+        <v>309</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>324</v>
+        <v>310</v>
       </c>
       <c r="C23" s="3">
         <v>4.0</v>
       </c>
-      <c r="D23" s="7" t="s">
-        <v>328</v>
+      <c r="D23" s="6" t="s">
+        <v>314</v>
       </c>
     </row>
     <row r="24">
-      <c r="A24" s="6" t="s">
-        <v>323</v>
+      <c r="A24" s="5" t="s">
+        <v>309</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>324</v>
+        <v>310</v>
       </c>
       <c r="C24" s="3">
         <v>5.0</v>
       </c>
-      <c r="D24" s="7" t="s">
-        <v>329</v>
+      <c r="D24" s="6" t="s">
+        <v>315</v>
       </c>
     </row>
     <row r="25">
-      <c r="A25" s="6" t="s">
-        <v>323</v>
+      <c r="A25" s="5" t="s">
+        <v>309</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>324</v>
+        <v>310</v>
       </c>
       <c r="C25" s="3">
         <v>6.0</v>
       </c>
-      <c r="D25" s="7" t="s">
-        <v>330</v>
+      <c r="D25" s="6" t="s">
+        <v>316</v>
       </c>
     </row>
     <row r="26">
-      <c r="A26" s="6" t="s">
-        <v>323</v>
+      <c r="A26" s="5" t="s">
+        <v>309</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>324</v>
+        <v>310</v>
       </c>
       <c r="C26" s="3">
         <v>7.0</v>
       </c>
-      <c r="D26" s="7" t="s">
-        <v>331</v>
+      <c r="D26" s="6" t="s">
+        <v>317</v>
       </c>
     </row>
     <row r="27">
-      <c r="A27" s="6" t="s">
-        <v>323</v>
+      <c r="A27" s="5" t="s">
+        <v>309</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>324</v>
+        <v>310</v>
       </c>
       <c r="C27" s="3">
         <v>8.0</v>
       </c>
-      <c r="D27" s="7" t="s">
-        <v>332</v>
+      <c r="D27" s="6" t="s">
+        <v>318</v>
       </c>
     </row>
     <row r="28">
@@ -5160,115 +5016,115 @@
       <c r="D28" s="1"/>
     </row>
     <row r="29">
-      <c r="A29" s="6" t="s">
-        <v>304</v>
+      <c r="A29" s="5" t="s">
+        <v>290</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>333</v>
+        <v>319</v>
       </c>
       <c r="C29" s="3">
         <v>1.0</v>
       </c>
-      <c r="D29" s="7" t="s">
-        <v>334</v>
+      <c r="D29" s="6" t="s">
+        <v>320</v>
       </c>
     </row>
     <row r="30">
-      <c r="A30" s="6" t="s">
-        <v>304</v>
+      <c r="A30" s="5" t="s">
+        <v>290</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>333</v>
+        <v>319</v>
       </c>
       <c r="C30" s="3">
         <v>2.0</v>
       </c>
-      <c r="D30" s="7" t="s">
-        <v>335</v>
+      <c r="D30" s="6" t="s">
+        <v>321</v>
       </c>
     </row>
     <row r="31">
-      <c r="A31" s="6" t="s">
-        <v>304</v>
+      <c r="A31" s="5" t="s">
+        <v>290</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>333</v>
+        <v>319</v>
       </c>
       <c r="C31" s="3">
         <v>3.0</v>
       </c>
-      <c r="D31" s="7" t="s">
-        <v>336</v>
+      <c r="D31" s="6" t="s">
+        <v>322</v>
       </c>
     </row>
     <row r="32">
-      <c r="A32" s="6" t="s">
-        <v>304</v>
+      <c r="A32" s="5" t="s">
+        <v>290</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>333</v>
+        <v>319</v>
       </c>
       <c r="C32" s="3">
         <v>4.0</v>
       </c>
-      <c r="D32" s="7" t="s">
-        <v>337</v>
+      <c r="D32" s="6" t="s">
+        <v>323</v>
       </c>
     </row>
     <row r="33">
-      <c r="A33" s="6" t="s">
-        <v>304</v>
+      <c r="A33" s="5" t="s">
+        <v>290</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>333</v>
+        <v>319</v>
       </c>
       <c r="C33" s="3">
         <v>5.0</v>
       </c>
-      <c r="D33" s="7" t="s">
-        <v>338</v>
+      <c r="D33" s="6" t="s">
+        <v>324</v>
       </c>
     </row>
     <row r="34">
-      <c r="A34" s="6" t="s">
-        <v>304</v>
+      <c r="A34" s="5" t="s">
+        <v>290</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>333</v>
+        <v>319</v>
       </c>
       <c r="C34" s="3">
         <v>6.0</v>
       </c>
-      <c r="D34" s="7" t="s">
-        <v>339</v>
+      <c r="D34" s="6" t="s">
+        <v>325</v>
       </c>
     </row>
     <row r="35">
-      <c r="A35" s="6" t="s">
-        <v>304</v>
+      <c r="A35" s="5" t="s">
+        <v>290</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>333</v>
+        <v>319</v>
       </c>
       <c r="C35" s="3">
         <v>7.0</v>
       </c>
-      <c r="D35" s="7" t="s">
-        <v>340</v>
+      <c r="D35" s="6" t="s">
+        <v>326</v>
       </c>
     </row>
     <row r="36">
-      <c r="A36" s="6" t="s">
-        <v>304</v>
+      <c r="A36" s="5" t="s">
+        <v>290</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>333</v>
+        <v>319</v>
       </c>
       <c r="C36" s="3">
         <v>8.0</v>
       </c>
-      <c r="D36" s="7" t="s">
-        <v>341</v>
+      <c r="D36" s="6" t="s">
+        <v>327</v>
       </c>
     </row>
     <row r="37">
@@ -5284,87 +5140,87 @@
       <c r="D38" s="1"/>
     </row>
     <row r="39">
-      <c r="A39" s="6" t="s">
-        <v>342</v>
+      <c r="A39" s="5" t="s">
+        <v>328</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>305</v>
+        <v>291</v>
       </c>
       <c r="C39" s="3">
         <v>1.0</v>
       </c>
-      <c r="D39" s="7" t="s">
-        <v>306</v>
+      <c r="D39" s="6" t="s">
+        <v>292</v>
       </c>
     </row>
     <row r="40">
-      <c r="A40" s="6" t="s">
-        <v>342</v>
+      <c r="A40" s="5" t="s">
+        <v>328</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>305</v>
+        <v>291</v>
       </c>
       <c r="C40" s="3">
         <v>2.0</v>
       </c>
-      <c r="D40" s="7" t="s">
-        <v>307</v>
+      <c r="D40" s="6" t="s">
+        <v>293</v>
       </c>
     </row>
     <row r="41">
-      <c r="A41" s="6" t="s">
-        <v>342</v>
+      <c r="A41" s="5" t="s">
+        <v>328</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>305</v>
+        <v>291</v>
       </c>
       <c r="C41" s="3">
         <v>3.0</v>
       </c>
-      <c r="D41" s="7" t="s">
-        <v>308</v>
+      <c r="D41" s="6" t="s">
+        <v>294</v>
       </c>
     </row>
     <row r="42">
-      <c r="A42" s="6" t="s">
-        <v>342</v>
+      <c r="A42" s="5" t="s">
+        <v>328</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>305</v>
+        <v>291</v>
       </c>
       <c r="C42" s="3">
         <v>4.0</v>
       </c>
-      <c r="D42" s="7" t="s">
-        <v>309</v>
+      <c r="D42" s="6" t="s">
+        <v>295</v>
       </c>
     </row>
     <row r="43">
-      <c r="A43" s="6" t="s">
-        <v>342</v>
+      <c r="A43" s="5" t="s">
+        <v>328</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>305</v>
+        <v>291</v>
       </c>
       <c r="C43" s="3">
         <v>5.0</v>
       </c>
-      <c r="D43" s="7" t="s">
-        <v>310</v>
+      <c r="D43" s="6" t="s">
+        <v>296</v>
       </c>
     </row>
     <row r="44">
-      <c r="A44" s="6" t="s">
-        <v>342</v>
+      <c r="A44" s="5" t="s">
+        <v>328</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>305</v>
+        <v>291</v>
       </c>
       <c r="C44" s="3">
         <v>6.0</v>
       </c>
-      <c r="D44" s="7" t="s">
-        <v>311</v>
+      <c r="D44" s="6" t="s">
+        <v>297</v>
       </c>
     </row>
     <row r="45">
@@ -5374,87 +5230,87 @@
       <c r="D45" s="1"/>
     </row>
     <row r="46">
-      <c r="A46" s="6" t="s">
-        <v>342</v>
+      <c r="A46" s="5" t="s">
+        <v>328</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>314</v>
+        <v>300</v>
       </c>
       <c r="C46" s="3">
         <v>1.0</v>
       </c>
-      <c r="D46" s="7" t="s">
-        <v>315</v>
+      <c r="D46" s="6" t="s">
+        <v>301</v>
       </c>
     </row>
     <row r="47">
-      <c r="A47" s="6" t="s">
-        <v>342</v>
+      <c r="A47" s="5" t="s">
+        <v>328</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>314</v>
+        <v>300</v>
       </c>
       <c r="C47" s="3">
         <v>2.0</v>
       </c>
-      <c r="D47" s="7" t="s">
-        <v>316</v>
+      <c r="D47" s="6" t="s">
+        <v>302</v>
       </c>
     </row>
     <row r="48">
-      <c r="A48" s="6" t="s">
-        <v>342</v>
+      <c r="A48" s="5" t="s">
+        <v>328</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>314</v>
+        <v>300</v>
       </c>
       <c r="C48" s="3">
         <v>3.0</v>
       </c>
-      <c r="D48" s="7" t="s">
-        <v>317</v>
+      <c r="D48" s="6" t="s">
+        <v>303</v>
       </c>
     </row>
     <row r="49">
-      <c r="A49" s="6" t="s">
-        <v>342</v>
+      <c r="A49" s="5" t="s">
+        <v>328</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>343</v>
+        <v>329</v>
       </c>
       <c r="C49" s="3">
         <v>1.0</v>
       </c>
-      <c r="D49" s="7" t="s">
-        <v>344</v>
+      <c r="D49" s="6" t="s">
+        <v>330</v>
       </c>
     </row>
     <row r="50">
-      <c r="A50" s="6" t="s">
-        <v>342</v>
+      <c r="A50" s="5" t="s">
+        <v>328</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>343</v>
+        <v>329</v>
       </c>
       <c r="C50" s="3">
         <v>2.0</v>
       </c>
-      <c r="D50" s="7" t="s">
-        <v>345</v>
+      <c r="D50" s="6" t="s">
+        <v>331</v>
       </c>
     </row>
     <row r="51">
-      <c r="A51" s="6" t="s">
-        <v>342</v>
+      <c r="A51" s="5" t="s">
+        <v>328</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>343</v>
+        <v>329</v>
       </c>
       <c r="C51" s="3">
         <v>3.0</v>
       </c>
-      <c r="D51" s="7" t="s">
-        <v>346</v>
+      <c r="D51" s="6" t="s">
+        <v>332</v>
       </c>
     </row>
     <row r="52">
@@ -5464,45 +5320,45 @@
       <c r="D52" s="1"/>
     </row>
     <row r="53">
-      <c r="A53" s="6" t="s">
-        <v>342</v>
+      <c r="A53" s="5" t="s">
+        <v>328</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>324</v>
+        <v>310</v>
       </c>
       <c r="C53" s="3">
         <v>1.0</v>
       </c>
-      <c r="D53" s="7" t="s">
-        <v>325</v>
+      <c r="D53" s="6" t="s">
+        <v>311</v>
       </c>
     </row>
     <row r="54">
-      <c r="A54" s="6" t="s">
-        <v>342</v>
+      <c r="A54" s="5" t="s">
+        <v>328</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>324</v>
+        <v>310</v>
       </c>
       <c r="C54" s="3">
         <v>2.0</v>
       </c>
-      <c r="D54" s="7" t="s">
-        <v>326</v>
+      <c r="D54" s="6" t="s">
+        <v>312</v>
       </c>
     </row>
     <row r="55">
-      <c r="A55" s="6" t="s">
-        <v>342</v>
+      <c r="A55" s="5" t="s">
+        <v>328</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>324</v>
+        <v>310</v>
       </c>
       <c r="C55" s="3">
         <v>3.0</v>
       </c>
-      <c r="D55" s="7" t="s">
-        <v>327</v>
+      <c r="D55" s="6" t="s">
+        <v>313</v>
       </c>
     </row>
     <row r="56">
@@ -5512,31 +5368,31 @@
       <c r="D56" s="1"/>
     </row>
     <row r="57">
-      <c r="A57" s="6" t="s">
-        <v>342</v>
+      <c r="A57" s="5" t="s">
+        <v>328</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>333</v>
+        <v>319</v>
       </c>
       <c r="C57" s="3">
         <v>1.0</v>
       </c>
-      <c r="D57" s="7" t="s">
-        <v>334</v>
+      <c r="D57" s="6" t="s">
+        <v>320</v>
       </c>
     </row>
     <row r="58">
-      <c r="A58" s="6" t="s">
-        <v>342</v>
+      <c r="A58" s="5" t="s">
+        <v>328</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>333</v>
+        <v>319</v>
       </c>
       <c r="C58" s="3">
         <v>2.0</v>
       </c>
-      <c r="D58" s="7" t="s">
-        <v>335</v>
+      <c r="D58" s="6" t="s">
+        <v>321</v>
       </c>
     </row>
     <row r="59">
@@ -5546,31 +5402,31 @@
       <c r="D59" s="1"/>
     </row>
     <row r="60">
-      <c r="A60" s="7" t="s">
-        <v>300</v>
+      <c r="A60" s="6" t="s">
+        <v>286</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>347</v>
+        <v>333</v>
       </c>
       <c r="C60" s="3">
         <v>1.0</v>
       </c>
-      <c r="D60" s="7" t="s">
-        <v>334</v>
+      <c r="D60" s="6" t="s">
+        <v>320</v>
       </c>
     </row>
     <row r="61">
-      <c r="A61" s="7" t="s">
-        <v>300</v>
+      <c r="A61" s="6" t="s">
+        <v>286</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>347</v>
+        <v>333</v>
       </c>
       <c r="C61" s="3">
         <v>2.0</v>
       </c>
-      <c r="D61" s="7" t="s">
-        <v>335</v>
+      <c r="D61" s="6" t="s">
+        <v>321</v>
       </c>
     </row>
     <row r="62">
@@ -5580,59 +5436,59 @@
       <c r="D62" s="1"/>
     </row>
     <row r="63">
-      <c r="A63" s="7" t="s">
-        <v>300</v>
+      <c r="A63" s="6" t="s">
+        <v>286</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>348</v>
+        <v>334</v>
       </c>
       <c r="C63" s="3">
         <v>1.0</v>
       </c>
-      <c r="D63" s="7" t="s">
-        <v>315</v>
+      <c r="D63" s="6" t="s">
+        <v>301</v>
       </c>
     </row>
     <row r="64">
-      <c r="A64" s="7" t="s">
-        <v>300</v>
+      <c r="A64" s="6" t="s">
+        <v>286</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>348</v>
+        <v>334</v>
       </c>
       <c r="C64" s="3">
         <v>2.0</v>
       </c>
-      <c r="D64" s="7" t="s">
-        <v>316</v>
+      <c r="D64" s="6" t="s">
+        <v>302</v>
       </c>
     </row>
     <row r="65">
-      <c r="A65" s="7" t="s">
-        <v>300</v>
+      <c r="A65" s="6" t="s">
+        <v>286</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>348</v>
+        <v>334</v>
       </c>
       <c r="C65" s="3">
         <v>3.0</v>
       </c>
-      <c r="D65" s="7" t="s">
-        <v>317</v>
+      <c r="D65" s="6" t="s">
+        <v>303</v>
       </c>
     </row>
     <row r="66">
-      <c r="A66" s="7" t="s">
-        <v>300</v>
+      <c r="A66" s="6" t="s">
+        <v>286</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>348</v>
+        <v>334</v>
       </c>
       <c r="C66" s="3">
         <v>4.0</v>
       </c>
-      <c r="D66" s="7" t="s">
-        <v>318</v>
+      <c r="D66" s="6" t="s">
+        <v>304</v>
       </c>
     </row>
     <row r="67">
@@ -5642,193 +5498,193 @@
       <c r="D67" s="1"/>
     </row>
     <row r="68">
-      <c r="A68" s="6" t="s">
-        <v>304</v>
+      <c r="A68" s="5" t="s">
+        <v>290</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>349</v>
+        <v>335</v>
       </c>
       <c r="C68" s="3">
         <v>1.0</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>289</v>
+        <v>336</v>
       </c>
     </row>
     <row r="69">
-      <c r="A69" s="6" t="s">
-        <v>304</v>
+      <c r="A69" s="5" t="s">
+        <v>290</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>349</v>
+        <v>335</v>
       </c>
       <c r="C69" s="3">
         <v>2.0</v>
       </c>
       <c r="D69" s="1" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" s="5" t="s">
         <v>290</v>
       </c>
-    </row>
-    <row r="70">
-      <c r="A70" s="6" t="s">
-        <v>304</v>
-      </c>
       <c r="B70" s="1" t="s">
-        <v>349</v>
+        <v>335</v>
       </c>
       <c r="C70" s="3">
         <v>3.0</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>291</v>
+        <v>338</v>
       </c>
     </row>
     <row r="71">
-      <c r="A71" s="6" t="s">
-        <v>304</v>
+      <c r="A71" s="5" t="s">
+        <v>290</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>349</v>
+        <v>335</v>
       </c>
       <c r="C71" s="3">
         <v>4.0</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>292</v>
+        <v>339</v>
       </c>
     </row>
     <row r="72">
-      <c r="A72" s="6" t="s">
-        <v>304</v>
+      <c r="A72" s="5" t="s">
+        <v>290</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>349</v>
+        <v>335</v>
       </c>
       <c r="C72" s="3">
         <v>5.0</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>293</v>
+        <v>340</v>
       </c>
     </row>
     <row r="73">
-      <c r="A73" s="6" t="s">
-        <v>304</v>
+      <c r="A73" s="5" t="s">
+        <v>290</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>349</v>
+        <v>335</v>
       </c>
       <c r="C73" s="3">
         <v>6.0</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>294</v>
+        <v>341</v>
       </c>
     </row>
     <row r="74">
-      <c r="A74" s="6" t="s">
-        <v>304</v>
+      <c r="A74" s="5" t="s">
+        <v>290</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>349</v>
+        <v>335</v>
       </c>
       <c r="C74" s="3">
         <v>7.0</v>
       </c>
       <c r="D74" s="1" t="s">
-        <v>295</v>
+        <v>342</v>
       </c>
     </row>
     <row r="75">
-      <c r="A75" s="6" t="s">
-        <v>304</v>
+      <c r="A75" s="5" t="s">
+        <v>290</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>349</v>
+        <v>335</v>
       </c>
       <c r="C75" s="3">
         <v>8.0</v>
       </c>
-      <c r="D75" s="5" t="s">
-        <v>296</v>
+      <c r="D75" s="7" t="s">
+        <v>343</v>
       </c>
     </row>
     <row r="76">
-      <c r="A76" s="6" t="s">
-        <v>304</v>
+      <c r="A76" s="5" t="s">
+        <v>290</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>349</v>
+        <v>335</v>
       </c>
       <c r="C76" s="3">
         <v>9.0</v>
       </c>
       <c r="D76" s="1" t="s">
-        <v>297</v>
+        <v>344</v>
       </c>
     </row>
     <row r="77">
-      <c r="A77" s="6" t="s">
-        <v>304</v>
+      <c r="A77" s="5" t="s">
+        <v>290</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>349</v>
+        <v>335</v>
       </c>
       <c r="C77" s="3">
         <v>10.0</v>
       </c>
       <c r="D77" s="1" t="s">
-        <v>298</v>
+        <v>345</v>
       </c>
     </row>
     <row r="78">
-      <c r="A78" s="6" t="s">
-        <v>304</v>
+      <c r="A78" s="5" t="s">
+        <v>290</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>349</v>
+        <v>335</v>
       </c>
       <c r="C78" s="3">
         <v>11.0</v>
       </c>
       <c r="D78" s="1" t="s">
-        <v>299</v>
+        <v>346</v>
       </c>
     </row>
     <row r="79">
-      <c r="A79" s="6" t="s">
-        <v>304</v>
+      <c r="A79" s="5" t="s">
+        <v>290</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>349</v>
+        <v>335</v>
       </c>
       <c r="C79" s="3">
         <v>12.0</v>
       </c>
       <c r="D79" s="1" t="s">
-        <v>299</v>
+        <v>346</v>
       </c>
     </row>
     <row r="80">
-      <c r="A80" s="6"/>
+      <c r="A80" s="5"/>
       <c r="B80" s="1"/>
       <c r="C80" s="1"/>
       <c r="D80" s="1"/>
     </row>
     <row r="81">
-      <c r="A81" s="6"/>
+      <c r="A81" s="5"/>
       <c r="B81" s="1"/>
       <c r="C81" s="1"/>
       <c r="D81" s="1"/>
     </row>
     <row r="82">
-      <c r="A82" s="6"/>
+      <c r="A82" s="5"/>
       <c r="B82" s="1"/>
       <c r="C82" s="1"/>
       <c r="D82" s="1"/>
     </row>
     <row r="83">
-      <c r="A83" s="6"/>
+      <c r="A83" s="5"/>
       <c r="B83" s="1"/>
       <c r="C83" s="1"/>
       <c r="D83" s="1"/>
@@ -11382,7 +11238,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
@@ -11399,13 +11255,13 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="4" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
     </row>
     <row r="2">
@@ -11413,10 +11269,10 @@
         <v>64.0</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>354</v>
+        <v>351</v>
       </c>
     </row>
     <row r="3">
@@ -11424,10 +11280,10 @@
         <v>39.0</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>355</v>
+        <v>352</v>
       </c>
     </row>
     <row r="4">
@@ -11435,10 +11291,10 @@
         <v>38.0</v>
       </c>
       <c r="B4" s="4" t="s">
+        <v>350</v>
+      </c>
+      <c r="C4" s="4" t="s">
         <v>353</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>356</v>
       </c>
     </row>
     <row r="5">
@@ -11449,7 +11305,7 @@
         <v>4</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
     </row>
     <row r="6">
@@ -11460,7 +11316,7 @@
         <v>4</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>356</v>
+        <v>353</v>
       </c>
     </row>
     <row r="7">
@@ -11471,7 +11327,7 @@
         <v>4</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
     </row>
     <row r="8">
@@ -11482,7 +11338,7 @@
         <v>5</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
     </row>
     <row r="9">
@@ -11493,7 +11349,7 @@
         <v>5</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
     </row>
     <row r="10">
@@ -11504,7 +11360,7 @@
         <v>5</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
     </row>
     <row r="11">
@@ -11515,7 +11371,7 @@
         <v>5</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>356</v>
+        <v>353</v>
       </c>
     </row>
     <row r="12">
@@ -11526,7 +11382,7 @@
         <v>5</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
     </row>
     <row r="13">
@@ -11537,7 +11393,7 @@
         <v>6</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
     </row>
     <row r="14">
@@ -11548,7 +11404,7 @@
         <v>6</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>362</v>
+        <v>359</v>
       </c>
     </row>
     <row r="15">
@@ -11559,7 +11415,7 @@
         <v>6</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>363</v>
+        <v>360</v>
       </c>
     </row>
     <row r="16">
@@ -11570,7 +11426,7 @@
         <v>6</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>364</v>
+        <v>361</v>
       </c>
     </row>
     <row r="17">
@@ -11581,7 +11437,7 @@
         <v>6</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>365</v>
+        <v>362</v>
       </c>
     </row>
     <row r="18">
@@ -11592,7 +11448,7 @@
         <v>6</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>366</v>
+        <v>363</v>
       </c>
     </row>
     <row r="19">
@@ -11603,7 +11459,7 @@
         <v>7</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>367</v>
+        <v>364</v>
       </c>
     </row>
     <row r="20">
@@ -11614,7 +11470,7 @@
         <v>7</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>368</v>
+        <v>365</v>
       </c>
     </row>
     <row r="21">
@@ -11625,7 +11481,7 @@
         <v>7</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>369</v>
+        <v>366</v>
       </c>
     </row>
     <row r="22">
@@ -11636,7 +11492,7 @@
         <v>7</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>370</v>
+        <v>367</v>
       </c>
     </row>
     <row r="23">
@@ -11647,7 +11503,7 @@
         <v>8</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>371</v>
+        <v>368</v>
       </c>
     </row>
     <row r="24">
@@ -11658,7 +11514,7 @@
         <v>8</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
     </row>
     <row r="25">
@@ -11669,7 +11525,7 @@
         <v>8</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
     </row>
     <row r="26">
@@ -11680,7 +11536,7 @@
         <v>8</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>374</v>
+        <v>371</v>
       </c>
     </row>
     <row r="27">
@@ -11691,7 +11547,7 @@
         <v>8</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>375</v>
+        <v>372</v>
       </c>
     </row>
     <row r="28">
@@ -11702,7 +11558,7 @@
         <v>8</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>376</v>
+        <v>373</v>
       </c>
     </row>
     <row r="29">
@@ -11713,7 +11569,7 @@
         <v>8</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
     </row>
     <row r="30">
@@ -11724,7 +11580,7 @@
         <v>8</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
     </row>
     <row r="31">
@@ -11735,7 +11591,7 @@
         <v>8</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
     </row>
     <row r="32">
@@ -11746,7 +11602,7 @@
         <v>8</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
     </row>
     <row r="33">
@@ -11757,7 +11613,7 @@
         <v>8</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>381</v>
+        <v>378</v>
       </c>
     </row>
     <row r="34">
@@ -11768,7 +11624,7 @@
         <v>8</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
     </row>
     <row r="35">
@@ -11779,7 +11635,7 @@
         <v>9</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
     </row>
     <row r="36">
@@ -11790,7 +11646,7 @@
         <v>9</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
     </row>
     <row r="37">
@@ -11801,7 +11657,7 @@
         <v>9</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>384</v>
+        <v>381</v>
       </c>
     </row>
     <row r="38">
@@ -11812,7 +11668,7 @@
         <v>9</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
     </row>
     <row r="39">
@@ -11823,7 +11679,7 @@
         <v>10</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
     </row>
     <row r="40">
@@ -11834,7 +11690,7 @@
         <v>11</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
     </row>
     <row r="41">
@@ -11845,7 +11701,7 @@
         <v>13</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>386</v>
+        <v>383</v>
       </c>
     </row>
     <row r="42">
@@ -11856,7 +11712,7 @@
         <v>13</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
     </row>
     <row r="43">
@@ -11867,7 +11723,7 @@
         <v>13</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
     </row>
     <row r="44">
@@ -11878,7 +11734,7 @@
         <v>14</v>
       </c>
       <c r="C44" s="4" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
     </row>
     <row r="45">
@@ -11889,7 +11745,7 @@
         <v>14</v>
       </c>
       <c r="C45" s="4" t="s">
-        <v>389</v>
+        <v>386</v>
       </c>
     </row>
     <row r="46">
@@ -11900,7 +11756,7 @@
         <v>15</v>
       </c>
       <c r="C46" s="4" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
     </row>
     <row r="47">
@@ -11911,7 +11767,7 @@
         <v>15</v>
       </c>
       <c r="C47" s="4" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
     </row>
     <row r="48">
@@ -11922,7 +11778,7 @@
         <v>15</v>
       </c>
       <c r="C48" s="4" t="s">
-        <v>392</v>
+        <v>389</v>
       </c>
     </row>
     <row r="49">
@@ -11933,7 +11789,7 @@
         <v>15</v>
       </c>
       <c r="C49" s="4" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
     </row>
     <row r="50">
@@ -11944,7 +11800,7 @@
         <v>15</v>
       </c>
       <c r="C50" s="4" t="s">
-        <v>393</v>
+        <v>390</v>
       </c>
     </row>
     <row r="51">
@@ -11955,7 +11811,7 @@
         <v>15</v>
       </c>
       <c r="C51" s="4" t="s">
-        <v>367</v>
+        <v>364</v>
       </c>
     </row>
     <row r="52">
@@ -11966,7 +11822,7 @@
         <v>16</v>
       </c>
       <c r="C52" s="4" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
     </row>
     <row r="53">
@@ -11977,7 +11833,7 @@
         <v>16</v>
       </c>
       <c r="C53" s="4" t="s">
-        <v>356</v>
+        <v>353</v>
       </c>
     </row>
     <row r="54">
@@ -11988,7 +11844,7 @@
         <v>16</v>
       </c>
       <c r="C54" s="4" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
     </row>
     <row r="55">
@@ -11999,7 +11855,7 @@
         <v>16</v>
       </c>
       <c r="C55" s="4" t="s">
-        <v>393</v>
+        <v>390</v>
       </c>
     </row>
     <row r="56">
@@ -12010,7 +11866,7 @@
         <v>16</v>
       </c>
       <c r="C56" s="4" t="s">
-        <v>367</v>
+        <v>364</v>
       </c>
     </row>
     <row r="57">
@@ -12021,7 +11877,7 @@
         <v>17</v>
       </c>
       <c r="C57" s="4" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
     </row>
     <row r="58">
@@ -12032,7 +11888,7 @@
         <v>17</v>
       </c>
       <c r="C58" s="4" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
     </row>
     <row r="59">
@@ -12043,7 +11899,7 @@
         <v>18</v>
       </c>
       <c r="C59" s="4" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
     </row>
     <row r="60">
@@ -12054,7 +11910,7 @@
         <v>18</v>
       </c>
       <c r="C60" s="4" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
     </row>
     <row r="61">
@@ -12065,7 +11921,7 @@
         <v>18</v>
       </c>
       <c r="C61" s="4" t="s">
-        <v>395</v>
+        <v>392</v>
       </c>
     </row>
     <row r="62">
@@ -12076,7 +11932,7 @@
         <v>19</v>
       </c>
       <c r="C62" s="4" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
     </row>
     <row r="63">
@@ -12087,7 +11943,7 @@
         <v>20</v>
       </c>
       <c r="C63" s="4" t="s">
-        <v>396</v>
+        <v>393</v>
       </c>
     </row>
     <row r="64">
@@ -12098,7 +11954,7 @@
         <v>20</v>
       </c>
       <c r="C64" s="4" t="s">
-        <v>397</v>
+        <v>394</v>
       </c>
     </row>
     <row r="65">
@@ -12109,7 +11965,7 @@
         <v>20</v>
       </c>
       <c r="C65" s="4" t="s">
-        <v>398</v>
+        <v>395</v>
       </c>
     </row>
     <row r="66">
@@ -12117,10 +11973,10 @@
         <v>29.0</v>
       </c>
       <c r="B66" s="4" t="s">
-        <v>399</v>
+        <v>396</v>
       </c>
       <c r="C66" s="4" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
     </row>
     <row r="67">
@@ -12131,7 +11987,7 @@
         <v>21</v>
       </c>
       <c r="C67" s="4" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
     </row>
     <row r="68">
@@ -12142,7 +11998,7 @@
         <v>22</v>
       </c>
       <c r="C68" s="4" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
     </row>
     <row r="69">
@@ -12153,7 +12009,7 @@
         <v>22</v>
       </c>
       <c r="C69" s="4" t="s">
-        <v>400</v>
+        <v>397</v>
       </c>
     </row>
     <row r="70">
@@ -12164,7 +12020,7 @@
         <v>23</v>
       </c>
       <c r="C70" s="4" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
     </row>
     <row r="71">
@@ -12175,7 +12031,7 @@
         <v>23</v>
       </c>
       <c r="C71" s="4" t="s">
-        <v>393</v>
+        <v>390</v>
       </c>
     </row>
     <row r="72">
@@ -12186,7 +12042,7 @@
         <v>23</v>
       </c>
       <c r="C72" s="4" t="s">
-        <v>367</v>
+        <v>364</v>
       </c>
     </row>
     <row r="73">
@@ -12197,7 +12053,7 @@
         <v>24</v>
       </c>
       <c r="C73" s="4" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
     </row>
     <row r="74">
@@ -12208,7 +12064,7 @@
         <v>24</v>
       </c>
       <c r="C74" s="4" t="s">
-        <v>401</v>
+        <v>398</v>
       </c>
     </row>
     <row r="75">
@@ -12219,7 +12075,7 @@
         <v>25</v>
       </c>
       <c r="C75" s="4" t="s">
-        <v>402</v>
+        <v>399</v>
       </c>
     </row>
     <row r="76">
@@ -12230,7 +12086,7 @@
         <v>25</v>
       </c>
       <c r="C76" s="4" t="s">
-        <v>367</v>
+        <v>364</v>
       </c>
     </row>
     <row r="77">
@@ -12238,10 +12094,10 @@
         <v>89.0</v>
       </c>
       <c r="B77" s="4" t="s">
-        <v>403</v>
+        <v>400</v>
       </c>
       <c r="C77" s="4" t="s">
-        <v>393</v>
+        <v>390</v>
       </c>
     </row>
     <row r="78">
@@ -12249,10 +12105,10 @@
         <v>65.0</v>
       </c>
       <c r="B78" s="4" t="s">
-        <v>403</v>
+        <v>400</v>
       </c>
       <c r="C78" s="4" t="s">
-        <v>367</v>
+        <v>364</v>
       </c>
     </row>
     <row r="79">
@@ -12263,7 +12119,7 @@
         <v>6</v>
       </c>
       <c r="C79" s="8" t="s">
-        <v>404</v>
+        <v>401</v>
       </c>
       <c r="D79" s="9"/>
       <c r="E79" s="9"/>
@@ -12297,7 +12153,7 @@
         <v>6</v>
       </c>
       <c r="C80" s="4" t="s">
-        <v>404</v>
+        <v>401</v>
       </c>
     </row>
     <row r="81">
@@ -12308,7 +12164,7 @@
         <v>22</v>
       </c>
       <c r="C81" s="4" t="s">
-        <v>405</v>
+        <v>402</v>
       </c>
     </row>
     <row r="82">
@@ -12319,7 +12175,7 @@
         <v>22</v>
       </c>
       <c r="C82" s="4" t="s">
-        <v>406</v>
+        <v>403</v>
       </c>
     </row>
     <row r="83">
@@ -12330,7 +12186,7 @@
         <v>7</v>
       </c>
       <c r="C83" s="4" t="s">
-        <v>407</v>
+        <v>404</v>
       </c>
     </row>
     <row r="84">
@@ -12341,7 +12197,7 @@
         <v>21</v>
       </c>
       <c r="C84" s="4" t="s">
-        <v>407</v>
+        <v>404</v>
       </c>
     </row>
     <row r="85">
@@ -12352,7 +12208,7 @@
         <v>11</v>
       </c>
       <c r="C85" s="4" t="s">
-        <v>407</v>
+        <v>404</v>
       </c>
     </row>
     <row r="86">
@@ -12360,10 +12216,10 @@
         <v>35.0</v>
       </c>
       <c r="B86" s="4" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="C86" s="4" t="s">
-        <v>407</v>
+        <v>404</v>
       </c>
     </row>
     <row r="87">
@@ -12374,7 +12230,7 @@
         <v>16</v>
       </c>
       <c r="C87" s="4" t="s">
-        <v>407</v>
+        <v>404</v>
       </c>
     </row>
     <row r="88">
@@ -12385,7 +12241,7 @@
         <v>25</v>
       </c>
       <c r="C88" s="4" t="s">
-        <v>407</v>
+        <v>404</v>
       </c>
     </row>
     <row r="89">
@@ -12396,7 +12252,7 @@
         <v>24</v>
       </c>
       <c r="C89" s="4" t="s">
-        <v>407</v>
+        <v>404</v>
       </c>
     </row>
     <row r="90">
@@ -12407,7 +12263,7 @@
         <v>15</v>
       </c>
       <c r="C90" s="4" t="s">
-        <v>407</v>
+        <v>404</v>
       </c>
     </row>
     <row r="91">
@@ -12418,7 +12274,7 @@
         <v>10</v>
       </c>
       <c r="C91" s="4" t="s">
-        <v>409</v>
+        <v>406</v>
       </c>
     </row>
     <row r="92">
@@ -12429,7 +12285,7 @@
         <v>10</v>
       </c>
       <c r="C92" s="4" t="s">
-        <v>410</v>
+        <v>407</v>
       </c>
     </row>
     <row r="93">
@@ -12440,7 +12296,7 @@
         <v>8</v>
       </c>
       <c r="C93" s="4" t="s">
-        <v>411</v>
+        <v>408</v>
       </c>
     </row>
     <row r="94">
@@ -12451,7 +12307,7 @@
         <v>8</v>
       </c>
       <c r="C94" s="4" t="s">
-        <v>412</v>
+        <v>409</v>
       </c>
     </row>
     <row r="95">
@@ -12462,7 +12318,7 @@
         <v>8</v>
       </c>
       <c r="C95" s="4" t="s">
-        <v>413</v>
+        <v>410</v>
       </c>
     </row>
     <row r="96">
@@ -12473,7 +12329,7 @@
         <v>8</v>
       </c>
       <c r="C96" s="4" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
     </row>
     <row r="97">
@@ -12484,7 +12340,7 @@
         <v>8</v>
       </c>
       <c r="C97" s="4" t="s">
-        <v>415</v>
+        <v>412</v>
       </c>
     </row>
     <row r="98">
@@ -12495,7 +12351,7 @@
         <v>8</v>
       </c>
       <c r="C98" s="4" t="s">
-        <v>416</v>
+        <v>413</v>
       </c>
     </row>
     <row r="99">
@@ -12506,7 +12362,7 @@
         <v>8</v>
       </c>
       <c r="C99" s="4" t="s">
-        <v>417</v>
+        <v>414</v>
       </c>
     </row>
     <row r="100">
@@ -12517,7 +12373,7 @@
         <v>8</v>
       </c>
       <c r="C100" s="4" t="s">
-        <v>418</v>
+        <v>415</v>
       </c>
     </row>
     <row r="101">
@@ -12528,7 +12384,7 @@
         <v>8</v>
       </c>
       <c r="C101" s="4" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
     </row>
     <row r="102">
@@ -12539,7 +12395,7 @@
         <v>8</v>
       </c>
       <c r="C102" s="4" t="s">
-        <v>420</v>
+        <v>417</v>
       </c>
     </row>
     <row r="103">
@@ -12550,7 +12406,7 @@
         <v>9</v>
       </c>
       <c r="C103" s="4" t="s">
-        <v>421</v>
+        <v>418</v>
       </c>
     </row>
     <row r="104">
@@ -12561,7 +12417,7 @@
         <v>16</v>
       </c>
       <c r="C104" s="4" t="s">
-        <v>421</v>
+        <v>418</v>
       </c>
     </row>
     <row r="105">
@@ -12572,7 +12428,7 @@
         <v>15</v>
       </c>
       <c r="C105" s="4" t="s">
-        <v>421</v>
+        <v>418</v>
       </c>
     </row>
     <row r="106">
@@ -12583,7 +12439,7 @@
         <v>13</v>
       </c>
       <c r="C106" s="4" t="s">
-        <v>422</v>
+        <v>419</v>
       </c>
     </row>
     <row r="107">
@@ -12594,7 +12450,7 @@
         <v>6</v>
       </c>
       <c r="C107" s="4" t="s">
-        <v>421</v>
+        <v>418</v>
       </c>
     </row>
     <row r="108">
@@ -12605,7 +12461,7 @@
         <v>7</v>
       </c>
       <c r="C108" s="4" t="s">
-        <v>421</v>
+        <v>418</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Big remap of file structure before moving it online
</commit_message>
<xml_diff>
--- a/Projects/Sung/Mapping Data/RTI Diagnostics Feed Info - Sung.xlsx
+++ b/Projects/Sung/Mapping Data/RTI Diagnostics Feed Info - Sung.xlsx
@@ -2941,1445 +2941,1054 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" min="3" max="3" width="34.0"/>
+    <col customWidth="1" min="2" max="2" width="34.0"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="4"/>
+      <c r="A1" s="4" t="s">
+        <v>166</v>
+      </c>
       <c r="B1" s="4" t="s">
-        <v>166</v>
-      </c>
-      <c r="C1" s="4" t="s">
         <v>167</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="B2" s="4">
+      <c r="A2" s="4">
         <v>0.0</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="B2" s="4" t="s">
         <v>168</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="B3" s="4">
+      <c r="A3" s="4">
         <v>1.0</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="B3" s="4" t="s">
         <v>169</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="B4" s="4">
+      <c r="A4" s="4">
         <v>2.0</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="B4" s="4" t="s">
         <v>170</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="B5" s="4">
+      <c r="A5" s="4">
         <v>3.0</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="B5" s="4" t="s">
         <v>170</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="B6" s="4">
+      <c r="A6" s="4">
         <v>4.0</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="B6" s="4" t="s">
         <v>170</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="B7" s="4">
+      <c r="A7" s="4">
         <v>5.0</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="B7" s="4" t="s">
         <v>170</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="B8" s="4">
+      <c r="A8" s="4">
         <v>6.0</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="B8" s="4" t="s">
         <v>170</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="B9" s="4">
+      <c r="A9" s="4">
         <v>7.0</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="B9" s="4" t="s">
         <v>170</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="B10" s="4">
+      <c r="A10" s="4">
         <v>8.0</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="B10" s="4" t="s">
         <v>170</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="B11" s="4">
+      <c r="A11" s="4">
         <v>9.0</v>
       </c>
-      <c r="C11" s="4" t="s">
+      <c r="B11" s="4" t="s">
         <v>170</v>
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="B12" s="4">
+      <c r="A12" s="4">
         <v>10.0</v>
       </c>
-      <c r="C12" s="4" t="s">
+      <c r="B12" s="4" t="s">
         <v>170</v>
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="B13" s="4">
+      <c r="A13" s="4">
         <v>11.0</v>
       </c>
-      <c r="C13" s="4" t="s">
+      <c r="B13" s="4" t="s">
         <v>170</v>
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="B14" s="4">
+      <c r="A14" s="4">
         <v>12.0</v>
       </c>
-      <c r="C14" s="4" t="s">
+      <c r="B14" s="4" t="s">
         <v>170</v>
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="B15" s="4">
+      <c r="A15" s="4">
         <v>13.0</v>
       </c>
-      <c r="C15" s="4" t="s">
+      <c r="B15" s="4" t="s">
         <v>170</v>
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="B16" s="4">
+      <c r="A16" s="4">
         <v>14.0</v>
       </c>
-      <c r="C16" s="4" t="s">
+      <c r="B16" s="4" t="s">
         <v>170</v>
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="B17" s="4">
+      <c r="A17" s="4">
         <v>15.0</v>
       </c>
-      <c r="C17" s="4" t="s">
+      <c r="B17" s="4" t="s">
         <v>170</v>
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="B18" s="4">
+      <c r="A18" s="4">
         <v>16.0</v>
       </c>
-      <c r="C18" s="4" t="s">
+      <c r="B18" s="4" t="s">
         <v>170</v>
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="B19" s="4">
+      <c r="A19" s="4">
         <v>17.0</v>
       </c>
-      <c r="C19" s="4" t="s">
+      <c r="B19" s="4" t="s">
         <v>170</v>
       </c>
     </row>
     <row r="20">
-      <c r="A20" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="B20" s="4">
+      <c r="A20" s="4">
         <v>18.0</v>
       </c>
-      <c r="C20" s="4" t="s">
+      <c r="B20" s="4" t="s">
         <v>170</v>
       </c>
     </row>
     <row r="21">
-      <c r="A21" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="B21" s="4">
+      <c r="A21" s="4">
         <v>19.0</v>
       </c>
-      <c r="C21" s="4" t="s">
+      <c r="B21" s="4" t="s">
         <v>170</v>
       </c>
     </row>
     <row r="22">
-      <c r="A22" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="B22" s="4">
+      <c r="A22" s="4">
         <v>20.0</v>
       </c>
-      <c r="C22" s="4" t="s">
+      <c r="B22" s="4" t="s">
         <v>171</v>
       </c>
     </row>
     <row r="23">
-      <c r="A23" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="B23" s="4">
+      <c r="A23" s="4">
         <v>21.0</v>
       </c>
-      <c r="C23" s="4" t="s">
+      <c r="B23" s="4" t="s">
         <v>172</v>
       </c>
     </row>
     <row r="24">
-      <c r="A24" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="B24" s="4">
+      <c r="A24" s="4">
         <v>22.0</v>
       </c>
-      <c r="C24" s="4" t="s">
+      <c r="B24" s="4" t="s">
         <v>173</v>
       </c>
     </row>
     <row r="25">
-      <c r="A25" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="B25" s="4">
+      <c r="A25" s="4">
         <v>23.0</v>
       </c>
-      <c r="C25" s="4" t="s">
+      <c r="B25" s="4" t="s">
         <v>174</v>
       </c>
     </row>
     <row r="26">
-      <c r="A26" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="B26" s="4">
+      <c r="A26" s="4">
         <v>24.0</v>
       </c>
-      <c r="C26" s="4" t="s">
+      <c r="B26" s="4" t="s">
         <v>175</v>
       </c>
     </row>
     <row r="27">
-      <c r="A27" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="B27" s="4">
+      <c r="A27" s="4">
         <v>25.0</v>
       </c>
-      <c r="C27" s="4" t="s">
+      <c r="B27" s="4" t="s">
         <v>176</v>
       </c>
     </row>
     <row r="28">
-      <c r="A28" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="B28" s="4">
+      <c r="A28" s="4">
         <v>26.0</v>
       </c>
-      <c r="C28" s="4" t="s">
+      <c r="B28" s="4" t="s">
         <v>177</v>
       </c>
     </row>
     <row r="29">
-      <c r="A29" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="B29" s="4">
+      <c r="A29" s="4">
         <v>27.0</v>
       </c>
-      <c r="C29" s="4" t="s">
+      <c r="B29" s="4" t="s">
         <v>178</v>
       </c>
     </row>
     <row r="30">
-      <c r="A30" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="B30" s="4">
+      <c r="A30" s="4">
         <v>28.0</v>
       </c>
-      <c r="C30" s="4" t="s">
+      <c r="B30" s="4" t="s">
         <v>179</v>
       </c>
     </row>
     <row r="31">
-      <c r="A31" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="B31" s="4">
+      <c r="A31" s="4">
         <v>29.0</v>
       </c>
-      <c r="C31" s="4" t="s">
+      <c r="B31" s="4" t="s">
         <v>180</v>
       </c>
     </row>
     <row r="32">
-      <c r="A32" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="B32" s="4">
+      <c r="A32" s="4">
         <v>30.0</v>
       </c>
-      <c r="C32" s="4" t="s">
+      <c r="B32" s="4" t="s">
         <v>181</v>
       </c>
     </row>
     <row r="33">
-      <c r="A33" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="B33" s="4">
+      <c r="A33" s="4">
         <v>31.0</v>
       </c>
-      <c r="C33" s="4" t="s">
+      <c r="B33" s="4" t="s">
         <v>182</v>
       </c>
     </row>
     <row r="34">
-      <c r="A34" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="B34" s="4">
+      <c r="A34" s="4">
         <v>32.0</v>
       </c>
-      <c r="C34" s="4" t="s">
+      <c r="B34" s="4" t="s">
         <v>183</v>
       </c>
     </row>
     <row r="35">
-      <c r="A35" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="B35" s="4">
+      <c r="A35" s="4">
         <v>33.0</v>
       </c>
-      <c r="C35" s="4" t="s">
+      <c r="B35" s="4" t="s">
         <v>184</v>
       </c>
     </row>
     <row r="36">
-      <c r="A36" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="B36" s="4">
+      <c r="A36" s="4">
         <v>34.0</v>
       </c>
-      <c r="C36" s="4" t="s">
+      <c r="B36" s="4" t="s">
         <v>185</v>
       </c>
     </row>
     <row r="37">
-      <c r="A37" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="B37" s="4">
+      <c r="A37" s="4">
         <v>35.0</v>
       </c>
-      <c r="C37" s="4" t="s">
+      <c r="B37" s="4" t="s">
         <v>186</v>
       </c>
     </row>
     <row r="38">
-      <c r="A38" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="B38" s="4">
+      <c r="A38" s="4">
         <v>36.0</v>
       </c>
-      <c r="C38" s="4" t="s">
+      <c r="B38" s="4" t="s">
         <v>187</v>
       </c>
     </row>
     <row r="39">
-      <c r="A39" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="B39" s="4">
+      <c r="A39" s="4">
         <v>37.0</v>
       </c>
-      <c r="C39" s="4" t="s">
+      <c r="B39" s="4" t="s">
         <v>188</v>
       </c>
     </row>
     <row r="40">
-      <c r="A40" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="B40" s="4">
+      <c r="A40" s="4">
         <v>38.0</v>
       </c>
-      <c r="C40" s="4" t="s">
+      <c r="B40" s="4" t="s">
         <v>189</v>
       </c>
     </row>
     <row r="41">
-      <c r="A41" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="B41" s="4">
+      <c r="A41" s="4">
         <v>39.0</v>
       </c>
-      <c r="C41" s="4" t="s">
+      <c r="B41" s="4" t="s">
         <v>190</v>
       </c>
     </row>
     <row r="42">
-      <c r="A42" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="B42" s="4">
+      <c r="A42" s="4">
         <v>40.0</v>
       </c>
-      <c r="C42" s="4" t="s">
+      <c r="B42" s="4" t="s">
         <v>191</v>
       </c>
     </row>
     <row r="43">
-      <c r="A43" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="B43" s="4">
+      <c r="A43" s="4">
         <v>41.0</v>
       </c>
-      <c r="C43" s="4" t="s">
+      <c r="B43" s="4" t="s">
         <v>192</v>
       </c>
     </row>
     <row r="44">
-      <c r="A44" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="B44" s="4">
+      <c r="A44" s="4">
         <v>42.0</v>
       </c>
-      <c r="C44" s="4" t="s">
+      <c r="B44" s="4" t="s">
         <v>193</v>
       </c>
     </row>
     <row r="45">
-      <c r="A45" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="B45" s="4">
+      <c r="A45" s="4">
         <v>43.0</v>
       </c>
-      <c r="C45" s="4" t="s">
+      <c r="B45" s="4" t="s">
         <v>194</v>
       </c>
     </row>
     <row r="46">
-      <c r="A46" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="B46" s="4">
+      <c r="A46" s="4">
         <v>44.0</v>
       </c>
-      <c r="C46" s="4" t="s">
+      <c r="B46" s="4" t="s">
         <v>194</v>
       </c>
     </row>
     <row r="47">
-      <c r="A47" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="B47" s="4">
+      <c r="A47" s="4">
         <v>45.0</v>
       </c>
-      <c r="C47" s="4" t="s">
+      <c r="B47" s="4" t="s">
         <v>194</v>
       </c>
     </row>
     <row r="48">
-      <c r="A48" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="B48" s="4">
+      <c r="A48" s="4">
         <v>46.0</v>
       </c>
-      <c r="C48" s="4" t="s">
+      <c r="B48" s="4" t="s">
         <v>195</v>
       </c>
     </row>
     <row r="49">
-      <c r="A49" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="B49" s="4">
+      <c r="A49" s="4">
         <v>47.0</v>
       </c>
-      <c r="C49" s="4" t="s">
+      <c r="B49" s="4" t="s">
         <v>196</v>
       </c>
     </row>
     <row r="50">
-      <c r="A50" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="B50" s="4">
+      <c r="A50" s="4">
         <v>48.0</v>
       </c>
-      <c r="C50" s="4" t="s">
+      <c r="B50" s="4" t="s">
         <v>197</v>
       </c>
     </row>
     <row r="51">
-      <c r="A51" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="B51" s="4">
+      <c r="A51" s="4">
         <v>49.0</v>
       </c>
-      <c r="C51" s="4" t="s">
+      <c r="B51" s="4" t="s">
         <v>197</v>
       </c>
     </row>
     <row r="52">
-      <c r="A52" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="B52" s="4">
+      <c r="A52" s="4">
         <v>50.0</v>
       </c>
-      <c r="C52" s="4" t="s">
+      <c r="B52" s="4" t="s">
         <v>198</v>
       </c>
     </row>
     <row r="53">
-      <c r="A53" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="B53" s="4">
+      <c r="A53" s="4">
         <v>51.0</v>
       </c>
-      <c r="C53" s="4" t="s">
+      <c r="B53" s="4" t="s">
         <v>199</v>
       </c>
     </row>
     <row r="54">
-      <c r="A54" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="B54" s="4">
+      <c r="A54" s="4">
         <v>52.0</v>
       </c>
-      <c r="C54" s="4" t="s">
+      <c r="B54" s="4" t="s">
         <v>200</v>
       </c>
     </row>
     <row r="55">
-      <c r="A55" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="B55" s="4">
+      <c r="A55" s="4">
         <v>53.0</v>
       </c>
-      <c r="C55" s="4" t="s">
+      <c r="B55" s="4" t="s">
         <v>201</v>
       </c>
     </row>
     <row r="56">
-      <c r="A56" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="B56" s="4">
+      <c r="A56" s="4">
         <v>54.0</v>
       </c>
-      <c r="C56" s="4" t="s">
+      <c r="B56" s="4" t="s">
         <v>202</v>
       </c>
     </row>
     <row r="57">
-      <c r="A57" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="B57" s="4">
+      <c r="A57" s="4">
         <v>55.0</v>
       </c>
-      <c r="C57" s="4" t="s">
+      <c r="B57" s="4" t="s">
         <v>203</v>
       </c>
     </row>
     <row r="58">
-      <c r="A58" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="B58" s="4">
+      <c r="A58" s="4">
         <v>56.0</v>
       </c>
-      <c r="C58" s="4" t="s">
+      <c r="B58" s="4" t="s">
         <v>204</v>
       </c>
     </row>
     <row r="59">
-      <c r="A59" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="B59" s="4">
+      <c r="A59" s="4">
         <v>57.0</v>
       </c>
-      <c r="C59" s="4" t="s">
+      <c r="B59" s="4" t="s">
         <v>205</v>
       </c>
     </row>
     <row r="60">
-      <c r="A60" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="B60" s="4">
+      <c r="A60" s="4">
         <v>58.0</v>
       </c>
-      <c r="C60" s="4" t="s">
+      <c r="B60" s="4" t="s">
         <v>170</v>
       </c>
     </row>
     <row r="61">
-      <c r="A61" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="B61" s="4">
+      <c r="A61" s="4">
         <v>59.0</v>
       </c>
-      <c r="C61" s="4" t="s">
+      <c r="B61" s="4" t="s">
         <v>206</v>
       </c>
     </row>
     <row r="62">
-      <c r="A62" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="B62" s="4">
+      <c r="A62" s="4">
         <v>60.0</v>
       </c>
-      <c r="C62" s="4" t="s">
+      <c r="B62" s="4" t="s">
         <v>170</v>
       </c>
     </row>
     <row r="63">
-      <c r="A63" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="B63" s="4">
+      <c r="A63" s="4">
         <v>61.0</v>
       </c>
-      <c r="C63" s="4" t="s">
+      <c r="B63" s="4" t="s">
         <v>207</v>
       </c>
     </row>
     <row r="64">
-      <c r="A64" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="B64" s="4">
+      <c r="A64" s="4">
         <v>62.0</v>
       </c>
-      <c r="C64" s="4" t="s">
+      <c r="B64" s="4" t="s">
         <v>208</v>
       </c>
     </row>
     <row r="65">
-      <c r="A65" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="B65" s="4">
+      <c r="A65" s="4">
         <v>63.0</v>
       </c>
-      <c r="C65" s="4" t="s">
+      <c r="B65" s="4" t="s">
         <v>209</v>
       </c>
     </row>
     <row r="66">
-      <c r="A66" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="B66" s="4">
+      <c r="A66" s="4">
         <v>64.0</v>
       </c>
-      <c r="C66" s="4" t="s">
+      <c r="B66" s="4" t="s">
         <v>210</v>
       </c>
     </row>
     <row r="67">
-      <c r="A67" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="B67" s="4">
+      <c r="A67" s="4">
         <v>65.0</v>
       </c>
-      <c r="C67" s="4" t="s">
+      <c r="B67" s="4" t="s">
         <v>211</v>
       </c>
     </row>
     <row r="68">
-      <c r="A68" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="B68" s="4">
+      <c r="A68" s="4">
         <v>66.0</v>
       </c>
-      <c r="C68" s="4" t="s">
+      <c r="B68" s="4" t="s">
         <v>212</v>
       </c>
     </row>
     <row r="69">
-      <c r="A69" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="B69" s="4">
+      <c r="A69" s="4">
         <v>67.0</v>
       </c>
-      <c r="C69" s="4" t="s">
+      <c r="B69" s="4" t="s">
         <v>213</v>
       </c>
     </row>
     <row r="70">
-      <c r="A70" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="B70" s="4">
+      <c r="A70" s="4">
         <v>68.0</v>
       </c>
-      <c r="C70" s="4" t="s">
+      <c r="B70" s="4" t="s">
         <v>170</v>
       </c>
     </row>
     <row r="71">
-      <c r="A71" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="B71" s="4">
+      <c r="A71" s="4">
         <v>69.0</v>
       </c>
-      <c r="C71" s="4" t="s">
+      <c r="B71" s="4" t="s">
         <v>170</v>
       </c>
     </row>
     <row r="72">
-      <c r="A72" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="B72" s="4">
+      <c r="A72" s="4">
         <v>70.0</v>
       </c>
-      <c r="C72" s="4" t="s">
+      <c r="B72" s="4" t="s">
         <v>170</v>
       </c>
     </row>
     <row r="73">
-      <c r="A73" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="B73" s="4">
+      <c r="A73" s="4">
         <v>71.0</v>
       </c>
-      <c r="C73" s="4" t="s">
+      <c r="B73" s="4" t="s">
         <v>170</v>
       </c>
     </row>
     <row r="74">
-      <c r="A74" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="B74" s="4">
+      <c r="A74" s="4">
         <v>72.0</v>
       </c>
-      <c r="C74" s="4" t="s">
+      <c r="B74" s="4" t="s">
         <v>214</v>
       </c>
     </row>
     <row r="75">
-      <c r="A75" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="B75" s="4">
+      <c r="A75" s="4">
         <v>73.0</v>
       </c>
-      <c r="C75" s="4" t="s">
+      <c r="B75" s="4" t="s">
         <v>215</v>
       </c>
     </row>
     <row r="76">
-      <c r="A76" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="B76" s="4">
+      <c r="A76" s="4">
         <v>74.0</v>
       </c>
-      <c r="C76" s="4" t="s">
+      <c r="B76" s="4" t="s">
         <v>216</v>
       </c>
     </row>
     <row r="77">
-      <c r="A77" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="B77" s="4">
+      <c r="A77" s="4">
         <v>75.0</v>
       </c>
-      <c r="C77" s="4" t="s">
+      <c r="B77" s="4" t="s">
         <v>217</v>
       </c>
     </row>
     <row r="78">
-      <c r="A78" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="B78" s="4">
+      <c r="A78" s="4">
         <v>76.0</v>
       </c>
-      <c r="C78" s="4" t="s">
+      <c r="B78" s="4" t="s">
         <v>218</v>
       </c>
     </row>
     <row r="79">
-      <c r="A79" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="B79" s="4">
+      <c r="A79" s="4">
         <v>77.0</v>
       </c>
-      <c r="C79" s="4" t="s">
+      <c r="B79" s="4" t="s">
         <v>219</v>
       </c>
     </row>
     <row r="80">
-      <c r="A80" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="B80" s="4">
+      <c r="A80" s="4">
         <v>78.0</v>
       </c>
-      <c r="C80" s="4" t="s">
+      <c r="B80" s="4" t="s">
         <v>220</v>
       </c>
     </row>
     <row r="81">
-      <c r="A81" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="B81" s="4">
+      <c r="A81" s="4">
         <v>79.0</v>
       </c>
-      <c r="C81" s="4" t="s">
+      <c r="B81" s="4" t="s">
         <v>221</v>
       </c>
     </row>
     <row r="82">
-      <c r="A82" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="B82" s="4">
+      <c r="A82" s="4">
         <v>80.0</v>
       </c>
-      <c r="C82" s="4" t="s">
+      <c r="B82" s="4" t="s">
         <v>222</v>
       </c>
     </row>
     <row r="83">
-      <c r="A83" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="B83" s="4">
+      <c r="A83" s="4">
         <v>81.0</v>
       </c>
-      <c r="C83" s="4" t="s">
+      <c r="B83" s="4" t="s">
         <v>223</v>
       </c>
     </row>
     <row r="84">
-      <c r="A84" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="B84" s="4">
+      <c r="A84" s="4">
         <v>82.0</v>
       </c>
-      <c r="C84" s="4" t="s">
+      <c r="B84" s="4" t="s">
         <v>224</v>
       </c>
     </row>
     <row r="85">
-      <c r="A85" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="B85" s="4">
+      <c r="A85" s="4">
         <v>83.0</v>
       </c>
-      <c r="C85" s="4" t="s">
+      <c r="B85" s="4" t="s">
         <v>225</v>
       </c>
     </row>
     <row r="86">
-      <c r="A86" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="B86" s="4">
+      <c r="A86" s="4">
         <v>84.0</v>
       </c>
-      <c r="C86" s="4" t="s">
+      <c r="B86" s="4" t="s">
         <v>226</v>
       </c>
     </row>
     <row r="87">
-      <c r="A87" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="B87" s="4">
+      <c r="A87" s="4">
         <v>85.0</v>
       </c>
-      <c r="C87" s="4" t="s">
+      <c r="B87" s="4" t="s">
         <v>227</v>
       </c>
     </row>
     <row r="88">
-      <c r="A88" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="B88" s="4">
+      <c r="A88" s="4">
         <v>86.0</v>
       </c>
-      <c r="C88" s="4" t="s">
+      <c r="B88" s="4" t="s">
         <v>228</v>
       </c>
     </row>
     <row r="89">
-      <c r="A89" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="B89" s="4">
+      <c r="A89" s="4">
         <v>87.0</v>
       </c>
-      <c r="C89" s="4" t="s">
+      <c r="B89" s="4" t="s">
         <v>229</v>
       </c>
     </row>
     <row r="90">
-      <c r="A90" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="B90" s="4">
+      <c r="A90" s="4">
         <v>88.0</v>
       </c>
-      <c r="C90" s="4" t="s">
+      <c r="B90" s="4" t="s">
         <v>230</v>
       </c>
     </row>
     <row r="91">
-      <c r="A91" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="B91" s="4">
+      <c r="A91" s="4">
         <v>89.0</v>
       </c>
-      <c r="C91" s="4" t="s">
+      <c r="B91" s="4" t="s">
         <v>231</v>
       </c>
     </row>
     <row r="92">
-      <c r="A92" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="B92" s="4">
+      <c r="A92" s="4">
         <v>90.0</v>
       </c>
-      <c r="C92" s="4" t="s">
+      <c r="B92" s="4" t="s">
         <v>232</v>
       </c>
     </row>
     <row r="93">
-      <c r="A93" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="B93" s="4">
+      <c r="A93" s="4">
         <v>91.0</v>
       </c>
-      <c r="C93" s="4" t="s">
+      <c r="B93" s="4" t="s">
         <v>233</v>
       </c>
     </row>
     <row r="94">
-      <c r="A94" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="B94" s="4">
+      <c r="A94" s="4">
         <v>92.0</v>
       </c>
-      <c r="C94" s="4" t="s">
+      <c r="B94" s="4" t="s">
         <v>234</v>
       </c>
     </row>
     <row r="95">
-      <c r="A95" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="B95" s="4">
+      <c r="A95" s="4">
         <v>93.0</v>
       </c>
-      <c r="C95" s="4" t="s">
+      <c r="B95" s="4" t="s">
         <v>234</v>
       </c>
     </row>
     <row r="96">
-      <c r="A96" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="B96" s="4">
+      <c r="A96" s="4">
         <v>94.0</v>
       </c>
-      <c r="C96" s="4" t="s">
+      <c r="B96" s="4" t="s">
         <v>235</v>
       </c>
     </row>
     <row r="97">
-      <c r="A97" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="B97" s="4">
+      <c r="A97" s="4">
         <v>95.0</v>
       </c>
-      <c r="C97" s="4" t="s">
+      <c r="B97" s="4" t="s">
         <v>236</v>
       </c>
     </row>
     <row r="98">
-      <c r="A98" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="B98" s="4">
+      <c r="A98" s="4">
         <v>96.0</v>
       </c>
-      <c r="C98" s="4" t="s">
+      <c r="B98" s="4" t="s">
         <v>237</v>
       </c>
     </row>
     <row r="99">
-      <c r="A99" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="B99" s="4">
+      <c r="A99" s="4">
         <v>97.0</v>
       </c>
-      <c r="C99" s="4" t="s">
+      <c r="B99" s="4" t="s">
         <v>238</v>
       </c>
     </row>
     <row r="100">
-      <c r="A100" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="B100" s="4">
+      <c r="A100" s="4">
         <v>98.0</v>
       </c>
-      <c r="C100" s="4" t="s">
+      <c r="B100" s="4" t="s">
         <v>239</v>
       </c>
     </row>
     <row r="101">
-      <c r="A101" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="B101" s="4">
+      <c r="A101" s="4">
         <v>99.0</v>
       </c>
-      <c r="C101" s="4" t="s">
+      <c r="B101" s="4" t="s">
         <v>240</v>
       </c>
     </row>
     <row r="102">
-      <c r="A102" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="B102" s="4">
+      <c r="A102" s="4">
         <v>100.0</v>
       </c>
-      <c r="C102" s="4" t="s">
+      <c r="B102" s="4" t="s">
         <v>241</v>
       </c>
     </row>
     <row r="103">
-      <c r="A103" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="B103" s="4">
+      <c r="A103" s="4">
         <v>101.0</v>
       </c>
-      <c r="C103" s="4" t="s">
+      <c r="B103" s="4" t="s">
         <v>242</v>
       </c>
     </row>
     <row r="104">
-      <c r="A104" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="B104" s="4">
+      <c r="A104" s="4">
         <v>102.0</v>
       </c>
-      <c r="C104" s="4" t="s">
+      <c r="B104" s="4" t="s">
         <v>243</v>
       </c>
     </row>
     <row r="105">
-      <c r="A105" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="B105" s="4">
+      <c r="A105" s="4">
         <v>103.0</v>
       </c>
-      <c r="C105" s="4" t="s">
+      <c r="B105" s="4" t="s">
         <v>244</v>
       </c>
     </row>
     <row r="106">
-      <c r="A106" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="B106" s="4">
+      <c r="A106" s="4">
         <v>104.0</v>
       </c>
-      <c r="C106" s="4" t="s">
+      <c r="B106" s="4" t="s">
         <v>245</v>
       </c>
     </row>
     <row r="107">
-      <c r="A107" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="B107" s="4">
+      <c r="A107" s="4">
         <v>105.0</v>
       </c>
-      <c r="C107" s="4" t="s">
+      <c r="B107" s="4" t="s">
         <v>246</v>
       </c>
     </row>
     <row r="108">
-      <c r="A108" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="B108" s="4">
+      <c r="A108" s="4">
         <v>106.0</v>
       </c>
-      <c r="C108" s="4" t="s">
+      <c r="B108" s="4" t="s">
         <v>247</v>
       </c>
     </row>
     <row r="109">
-      <c r="A109" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="B109" s="4">
+      <c r="A109" s="4">
         <v>107.0</v>
       </c>
-      <c r="C109" s="4" t="s">
+      <c r="B109" s="4" t="s">
         <v>248</v>
       </c>
     </row>
     <row r="110">
-      <c r="A110" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="B110" s="4">
+      <c r="A110" s="4">
         <v>108.0</v>
       </c>
-      <c r="C110" s="4" t="s">
+      <c r="B110" s="4" t="s">
         <v>249</v>
       </c>
     </row>
     <row r="111">
-      <c r="A111" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="B111" s="4">
+      <c r="A111" s="4">
         <v>109.0</v>
       </c>
-      <c r="C111" s="4" t="s">
+      <c r="B111" s="4" t="s">
         <v>250</v>
       </c>
     </row>
     <row r="112">
-      <c r="A112" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="B112" s="4">
+      <c r="A112" s="4">
         <v>110.0</v>
       </c>
-      <c r="C112" s="4" t="s">
+      <c r="B112" s="4" t="s">
         <v>251</v>
       </c>
     </row>
     <row r="113">
-      <c r="A113" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="B113" s="4">
+      <c r="A113" s="4">
         <v>111.0</v>
       </c>
-      <c r="C113" s="4" t="s">
+      <c r="B113" s="4" t="s">
         <v>252</v>
       </c>
     </row>
     <row r="114">
-      <c r="A114" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="B114" s="4">
+      <c r="A114" s="4">
         <v>112.0</v>
       </c>
-      <c r="C114" s="4" t="s">
+      <c r="B114" s="4" t="s">
         <v>253</v>
       </c>
     </row>
     <row r="115">
-      <c r="A115" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="B115" s="4">
+      <c r="A115" s="4">
         <v>113.0</v>
       </c>
-      <c r="C115" s="4" t="s">
+      <c r="B115" s="4" t="s">
         <v>254</v>
       </c>
     </row>
     <row r="116">
-      <c r="A116" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="B116" s="4">
+      <c r="A116" s="4">
         <v>114.0</v>
       </c>
-      <c r="C116" s="4" t="s">
+      <c r="B116" s="4" t="s">
         <v>255</v>
       </c>
     </row>
     <row r="117">
-      <c r="A117" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="B117" s="4">
+      <c r="A117" s="4">
         <v>115.0</v>
       </c>
-      <c r="C117" s="4" t="s">
+      <c r="B117" s="4" t="s">
         <v>256</v>
       </c>
     </row>
     <row r="118">
-      <c r="A118" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="B118" s="4">
+      <c r="A118" s="4">
         <v>116.0</v>
       </c>
-      <c r="C118" s="4" t="s">
+      <c r="B118" s="4" t="s">
         <v>257</v>
       </c>
     </row>
     <row r="119">
-      <c r="A119" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="B119" s="4">
+      <c r="A119" s="4">
         <v>117.0</v>
       </c>
-      <c r="C119" s="4" t="s">
+      <c r="B119" s="4" t="s">
         <v>258</v>
       </c>
     </row>
     <row r="120">
-      <c r="A120" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="B120" s="4">
+      <c r="A120" s="4">
         <v>118.0</v>
       </c>
-      <c r="C120" s="4" t="s">
+      <c r="B120" s="4" t="s">
         <v>259</v>
       </c>
     </row>
     <row r="121">
-      <c r="A121" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="B121" s="4">
+      <c r="A121" s="4">
         <v>119.0</v>
       </c>
-      <c r="C121" s="4" t="s">
+      <c r="B121" s="4" t="s">
         <v>260</v>
       </c>
     </row>
     <row r="122">
-      <c r="A122" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="B122" s="4">
+      <c r="A122" s="4">
         <v>120.0</v>
       </c>
-      <c r="C122" s="4" t="s">
+      <c r="B122" s="4" t="s">
         <v>261</v>
       </c>
     </row>
     <row r="123">
-      <c r="A123" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="B123" s="4">
+      <c r="A123" s="4">
         <v>121.0</v>
       </c>
-      <c r="C123" s="4" t="s">
+      <c r="B123" s="4" t="s">
         <v>262</v>
       </c>
     </row>
     <row r="124">
-      <c r="A124" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="B124" s="4">
+      <c r="A124" s="4">
         <v>122.0</v>
       </c>
-      <c r="C124" s="4" t="s">
+      <c r="B124" s="4" t="s">
         <v>263</v>
       </c>
     </row>
     <row r="125">
-      <c r="A125" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="B125" s="4">
+      <c r="A125" s="4">
         <v>123.0</v>
       </c>
-      <c r="C125" s="4" t="s">
+      <c r="B125" s="4" t="s">
         <v>264</v>
       </c>
     </row>
     <row r="126">
-      <c r="A126" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="B126" s="4">
+      <c r="A126" s="4">
         <v>124.0</v>
       </c>
-      <c r="C126" s="4" t="s">
+      <c r="B126" s="4" t="s">
         <v>265</v>
       </c>
     </row>
     <row r="127">
-      <c r="A127" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="B127" s="4">
+      <c r="A127" s="4">
         <v>125.0</v>
       </c>
-      <c r="C127" s="4" t="s">
+      <c r="B127" s="4" t="s">
         <v>266</v>
       </c>
     </row>
     <row r="128">
-      <c r="A128" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="B128" s="4">
+      <c r="A128" s="4">
         <v>126.0</v>
       </c>
-      <c r="C128" s="4" t="s">
+      <c r="B128" s="4" t="s">
         <v>267</v>
       </c>
     </row>
     <row r="129">
-      <c r="A129" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="B129" s="4">
+      <c r="A129" s="4">
         <v>127.0</v>
       </c>
-      <c r="C129" s="4" t="s">
+      <c r="B129" s="4" t="s">
         <v>268</v>
       </c>
     </row>
     <row r="130">
-      <c r="A130" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="B130" s="4">
+      <c r="A130" s="4">
         <v>128.0</v>
       </c>
-      <c r="C130" s="4" t="s">
+      <c r="B130" s="4" t="s">
         <v>269</v>
       </c>
     </row>
     <row r="131">
-      <c r="A131" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="B131" s="4">
+      <c r="A131" s="4">
         <v>129.0</v>
       </c>
-      <c r="C131" s="4" t="s">
+      <c r="B131" s="4" t="s">
         <v>270</v>
       </c>
     </row>

</xml_diff>